<commit_message>
implemented turma, class types + fitness function
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="961" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C07898A4-7EC5-46B4-8285-FC3909E48D34}"/>
+  <xr:revisionPtr revIDLastSave="963" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62E91487-33D4-4397-88F1-BA9616F2EB5C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="150">
   <si>
     <t>CURSO: ENGENHARIA DE SOFTWARE</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>GB922</t>
+  </si>
+  <si>
+    <t>AB122</t>
   </si>
 </sst>
 </file>
@@ -626,26 +629,10 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="7"/>
-          <bgColor theme="7"/>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -682,10 +669,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.79998168889431442"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <fgColor theme="7"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -818,10 +821,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
@@ -849,7 +848,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}" name="Table2" displayName="Table2" ref="B4:D52" totalsRowShown="0">
   <autoFilter ref="B4:D52" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:D52">
-    <sortCondition ref="D4:D52"/>
+    <sortCondition ref="C4:C52"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DA2ECD09-3FA6-4544-AE27-6E4A1304C0F4}" name="DISCIPLINA"/>
@@ -875,16 +874,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}" name="Table4" displayName="Table4" ref="I2:L35" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}" name="Table4" displayName="Table4" ref="I2:L35" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="I2:L35" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:L35">
     <sortCondition ref="L2:L35"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C8A0A278-3838-4995-8588-B07D13EA3EFD}" name="NOME" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D7D84DAB-D2AE-4879-9CEE-32E7CA42BC4C}" name="CR" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{60337C39-789F-4651-A8AB-E68BD1E538E3}" name="SL/B" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4DEB40D6-B26B-4C55-8BD0-3BE4E24E00B0}" name="ET" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C8A0A278-3838-4995-8588-B07D13EA3EFD}" name="NOME" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D7D84DAB-D2AE-4879-9CEE-32E7CA42BC4C}" name="CR" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{60337C39-789F-4651-A8AB-E68BD1E538E3}" name="SL/B" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4DEB40D6-B26B-4C55-8BD0-3BE4E24E00B0}" name="ET" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1155,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
@@ -2558,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177CF1B3-023B-4C26-8BA7-3BF936A39EC1}">
   <dimension ref="B1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2607,134 +2606,134 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2">
-        <v>11792</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="D7" s="2">
-        <v>11792</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="D8" s="2">
-        <v>11792</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2">
-        <v>12203</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D10" s="2">
-        <v>12274</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2">
-        <v>12274</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2">
-        <v>12274</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D13" s="2">
-        <v>13000</v>
+        <v>14616</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D14" s="2">
-        <v>13000</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2">
-        <v>13000</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D16" s="2">
-        <v>13000</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2">
-        <v>13034</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -2750,245 +2749,245 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2">
-        <v>13034</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D20" s="2">
-        <v>13034</v>
+        <v>12203</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="D21" s="2">
-        <v>13034</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="D22" s="2">
-        <v>13070</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="D23" s="2">
-        <v>13070</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="D24" s="2">
-        <v>14091</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2">
-        <v>14091</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D26" s="2">
-        <v>14472</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D27" s="2">
-        <v>14472</v>
+        <v>45000</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2">
-        <v>14472</v>
+        <v>13070</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D29" s="2">
-        <v>14472</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2">
-        <v>14472</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D31" s="2">
-        <v>14525</v>
+        <v>14091</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D32" s="2">
-        <v>14525</v>
+        <v>14091</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="D33" s="2">
-        <v>14525</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D34" s="2">
-        <v>14525</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="D35" s="2">
-        <v>14616</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D36" s="2">
-        <v>14642</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="D37" s="2">
-        <v>14642</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D38" s="2">
-        <v>14642</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D39" s="2">
-        <v>14642</v>
+        <v>13070</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="D40" s="2">
-        <v>14642</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
@@ -3015,112 +3014,112 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D43" s="2">
-        <v>14776</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D44" s="2">
-        <v>14776</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D45" s="2">
-        <v>14776</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D46" s="2">
-        <v>14875</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D47" s="2">
-        <v>14875</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D48" s="2">
-        <v>14875</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D49" s="2">
-        <v>45000</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D50" s="2">
-        <v>45000</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D51" s="2">
-        <v>45000</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="D52" s="2">
-        <v>45000</v>
+        <v>11792</v>
       </c>
     </row>
   </sheetData>
@@ -3323,7 +3322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71808F-48CA-4498-917A-4D75806DE602}">
   <dimension ref="B2:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
checked db, created constraints
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="963" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62E91487-33D4-4397-88F1-BA9616F2EB5C}"/>
+  <xr:revisionPtr revIDLastSave="968" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFC080DD-75C6-4232-B4ED-20752F50C8C1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="150">
   <si>
     <t>CURSO: ENGENHARIA DE SOFTWARE</t>
   </si>
@@ -598,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -623,6 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,11 +822,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:L42">
-    <sortCondition ref="J4:J42"/>
+    <sortCondition ref="G4:G42"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{9CD2D2FA-51BA-4A30-A0C5-D56FD2E46138}" name="DISCIPLINA" dataDxfId="18"/>
@@ -845,10 +850,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}" name="Table2" displayName="Table2" ref="B4:D52" totalsRowShown="0">
-  <autoFilter ref="B4:D52" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:D52">
-    <sortCondition ref="C4:C52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}" name="Table2" displayName="Table2" ref="B4:D51" totalsRowShown="0">
+  <autoFilter ref="B4:D51" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:D51">
+    <sortCondition ref="D4:D51"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DA2ECD09-3FA6-4544-AE27-6E4A1304C0F4}" name="DISCIPLINA"/>
@@ -1155,7 +1160,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,13 +1288,13 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -1298,62 +1303,62 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
         <v>73</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K7" s="2">
-        <v>11792</v>
+        <v>14472</v>
       </c>
       <c r="L7" s="5">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
         <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8" s="2">
-        <v>13034</v>
+        <v>14472</v>
       </c>
       <c r="L8" s="5">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1368,27 +1373,27 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
         <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9" s="2">
+        <v>45000</v>
+      </c>
+      <c r="L9" s="5">
         <v>1</v>
-      </c>
-      <c r="K9" s="2">
-        <v>13070</v>
-      </c>
-      <c r="L9" s="5">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1403,30 +1408,30 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="H10" t="s">
         <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K10" s="2">
-        <v>13070</v>
+        <v>14616</v>
       </c>
       <c r="L10" s="5">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -1438,62 +1443,62 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
         <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K11" s="2">
-        <v>11792</v>
+        <v>12274</v>
       </c>
       <c r="L11" s="5">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H12" t="s">
         <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K12" s="2">
-        <v>45000</v>
+        <v>14642</v>
       </c>
       <c r="L12" s="5">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1508,33 +1513,33 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H13" t="s">
         <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13" s="2">
-        <v>45000</v>
+        <v>14472</v>
       </c>
       <c r="L13" s="5">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -1543,138 +1548,138 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
         <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K14" s="2">
-        <v>45000</v>
+        <v>13034</v>
       </c>
       <c r="L14" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" t="s">
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
       <c r="K15" s="2">
-        <v>14472</v>
+        <v>12203</v>
       </c>
       <c r="L15" s="5">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
       <c r="K16" s="2">
-        <v>14472</v>
+        <v>11792</v>
       </c>
       <c r="L16" s="5">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="H17" t="s">
         <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K17" s="2">
-        <v>14472</v>
+        <v>13034</v>
       </c>
       <c r="L17" s="5">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -1683,27 +1688,27 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="H18" t="s">
         <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K18" s="2">
-        <v>14642</v>
+        <v>11792</v>
       </c>
       <c r="L18" s="5">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1715,33 +1720,33 @@
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
         <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K19" s="2">
-        <v>12203</v>
+        <v>14875</v>
       </c>
       <c r="L19" s="5">
-        <v>71</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -1750,30 +1755,30 @@
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="H20" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K20" s="2">
-        <v>14091</v>
+        <v>45000</v>
       </c>
       <c r="L20" s="5">
-        <v>53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -1788,27 +1793,27 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H21" t="s">
         <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K21" s="2">
-        <v>13034</v>
+        <v>45000</v>
       </c>
       <c r="L21" s="5">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -1823,62 +1828,62 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H22" t="s">
         <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K22" s="2">
-        <v>13034</v>
+        <v>13070</v>
       </c>
       <c r="L22" s="5">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" t="s">
+        <v>84</v>
+      </c>
+      <c r="J23">
         <v>1</v>
       </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" t="s">
-        <v>73</v>
-      </c>
-      <c r="I23" t="s">
-        <v>76</v>
-      </c>
-      <c r="J23">
-        <v>4</v>
-      </c>
       <c r="K23" s="2">
-        <v>13034</v>
+        <v>13070</v>
       </c>
       <c r="L23" s="5">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -1893,33 +1898,33 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
         <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K24" s="2">
-        <v>14091</v>
+        <v>14642</v>
       </c>
       <c r="L24" s="5">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -1928,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H25" t="s">
         <v>73</v>
@@ -1940,18 +1945,18 @@
         <v>4</v>
       </c>
       <c r="K25" s="2">
-        <v>14525</v>
+        <v>14091</v>
       </c>
       <c r="L25" s="5">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -1960,36 +1965,36 @@
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="H26" t="s">
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K26" s="2">
-        <v>14642</v>
+        <v>14091</v>
       </c>
       <c r="L26" s="5">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -1998,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="H27" t="s">
         <v>73</v>
@@ -2010,21 +2015,21 @@
         <v>5</v>
       </c>
       <c r="K27" s="2">
-        <v>12274</v>
+        <v>14642</v>
       </c>
       <c r="L27" s="5">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -2033,27 +2038,27 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>123</v>
+        <v>50</v>
       </c>
       <c r="H28" t="s">
         <v>73</v>
       </c>
       <c r="I28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J28">
         <v>5</v>
       </c>
       <c r="K28" s="2">
-        <v>14642</v>
+        <v>14875</v>
       </c>
       <c r="L28" s="5">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
@@ -2068,33 +2073,33 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H29" t="s">
         <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K29" s="2">
-        <v>14875</v>
+        <v>13000</v>
       </c>
       <c r="L29" s="5">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -2103,33 +2108,33 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s">
         <v>73</v>
       </c>
       <c r="I30" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K30" s="2">
-        <v>13034</v>
+        <v>14525</v>
       </c>
       <c r="L30" s="5">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -2138,33 +2143,33 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H31" t="s">
         <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K31" s="2">
-        <v>14525</v>
+        <v>45000</v>
       </c>
       <c r="L31" s="5">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -2173,27 +2178,27 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H32" t="s">
         <v>73</v>
       </c>
       <c r="I32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J32">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K32" s="2">
-        <v>14776</v>
+        <v>13070</v>
       </c>
       <c r="L32" s="5">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -2208,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H33" t="s">
         <v>73</v>
@@ -2217,56 +2222,56 @@
         <v>80</v>
       </c>
       <c r="J33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K33" s="2">
-        <v>45000</v>
+        <v>14642</v>
       </c>
       <c r="L33" s="5">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+      <c r="K34" s="2">
+        <v>14642</v>
+      </c>
+      <c r="L34" s="5">
         <v>11</v>
-      </c>
-      <c r="C34" s="1">
-        <v>2</v>
-      </c>
-      <c r="D34" s="1">
-        <v>2</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" t="s">
-        <v>53</v>
-      </c>
-      <c r="H34" t="s">
-        <v>73</v>
-      </c>
-      <c r="I34" t="s">
-        <v>81</v>
-      </c>
-      <c r="J34">
-        <v>6</v>
-      </c>
-      <c r="K34" s="2">
-        <v>13000</v>
-      </c>
-      <c r="L34" s="5">
-        <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -2278,33 +2283,33 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H35" t="s">
         <v>73</v>
       </c>
       <c r="I35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K35" s="2">
-        <v>14525</v>
+        <v>13034</v>
       </c>
       <c r="L35" s="5">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C36" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
@@ -2313,33 +2318,33 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="H36" t="s">
         <v>73</v>
       </c>
       <c r="I36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J36">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K36" s="2">
-        <v>14616</v>
+        <v>14525</v>
       </c>
       <c r="L36" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C37" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -2348,33 +2353,33 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H37" t="s">
         <v>73</v>
       </c>
       <c r="I37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J37">
         <v>7</v>
       </c>
       <c r="K37" s="2">
-        <v>14875</v>
+        <v>13000</v>
       </c>
       <c r="L37" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -2383,27 +2388,27 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="H38" t="s">
         <v>73</v>
       </c>
       <c r="I38" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J38">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K38" s="2">
-        <v>14642</v>
+        <v>13034</v>
       </c>
       <c r="L38" s="5">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -2418,33 +2423,33 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="H39" t="s">
         <v>73</v>
       </c>
       <c r="I39" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J39">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K39" s="2">
-        <v>13070</v>
+        <v>13034</v>
       </c>
       <c r="L39" s="5">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C40" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -2453,68 +2458,68 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H40" t="s">
         <v>73</v>
       </c>
       <c r="I40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J40">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K40" s="2">
-        <v>13000</v>
+        <v>14776</v>
       </c>
       <c r="L40" s="5">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>82</v>
+      </c>
+      <c r="J41">
+        <v>6</v>
+      </c>
+      <c r="K41" s="2">
+        <v>14525</v>
+      </c>
+      <c r="L41" s="5">
         <v>4</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
-      <c r="F41" s="1">
-        <v>0</v>
-      </c>
-      <c r="G41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I41" t="s">
-        <v>85</v>
-      </c>
-      <c r="J41">
-        <v>7</v>
-      </c>
-      <c r="K41" s="2">
-        <v>11792</v>
-      </c>
-      <c r="L41" s="5">
-        <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C42" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -2523,22 +2528,22 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="H42" t="s">
         <v>73</v>
       </c>
       <c r="I42" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K42" s="2">
-        <v>14642</v>
+        <v>11792</v>
       </c>
       <c r="L42" s="5">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2555,10 +2560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177CF1B3-023B-4C26-8BA7-3BF936A39EC1}">
-  <dimension ref="B1:K52"/>
+  <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2594,7 +2599,7 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="12" t="s">
         <v>117</v>
       </c>
       <c r="C5" t="s">
@@ -2606,134 +2611,134 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="D6" s="2">
-        <v>13034</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="D7" s="2">
-        <v>14525</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="D8" s="2">
-        <v>14776</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2">
-        <v>14472</v>
+        <v>12203</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2">
-        <v>14642</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2">
-        <v>14776</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2">
-        <v>45000</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="D13" s="2">
-        <v>14616</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2">
-        <v>12274</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2">
-        <v>14472</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D16" s="2">
-        <v>14642</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>107</v>
+      <c r="B17" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2">
-        <v>14875</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -2749,234 +2754,234 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="D19" s="2">
-        <v>14472</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2">
-        <v>12203</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="D21" s="2">
-        <v>11792</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="D22" s="2">
-        <v>13000</v>
+        <v>13070</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>58</v>
       </c>
       <c r="D23" s="2">
-        <v>13034</v>
+        <v>13070</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2">
-        <v>11792</v>
+        <v>14091</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D25" s="2">
-        <v>14875</v>
+        <v>14091</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2">
-        <v>45000</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2">
-        <v>45000</v>
+        <v>14472</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D28" s="2">
-        <v>13070</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D29" s="2">
-        <v>14642</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2">
-        <v>14642</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>109</v>
+      <c r="B31" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D31" s="2">
-        <v>14091</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D32" s="2">
-        <v>14091</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
       <c r="D33" s="2">
-        <v>14642</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D34" s="2">
-        <v>14875</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="D35" s="2">
-        <v>13000</v>
+        <v>14616</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D36" s="2">
-        <v>14525</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="D37" s="2">
-        <v>45000</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D38" s="2">
-        <v>12274</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="D39" s="2">
-        <v>13070</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
@@ -2987,139 +2992,128 @@
         <v>59</v>
       </c>
       <c r="D40" s="2">
-        <v>12274</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D41" s="2">
         <v>14642</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>122</v>
+      <c r="B42" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" s="2">
-        <v>14642</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D43" s="2">
-        <v>13034</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" s="2">
-        <v>14472</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D45" s="2">
-        <v>14525</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" s="2">
-        <v>13000</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D47" s="2">
-        <v>13034</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D48" s="2">
-        <v>14472</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D49" s="2">
-        <v>13000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C50" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D50" s="2">
-        <v>14776</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D51" s="2">
-        <v>14525</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>139</v>
-      </c>
-      <c r="C52" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" s="2">
-        <v>11792</v>
+        <v>45000</v>
       </c>
     </row>
   </sheetData>
@@ -3141,8 +3135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E06C8D-EBEC-4F83-9AB8-8954035C71B9}">
   <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
rewrote script except fitness function (todo)
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="968" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFC080DD-75C6-4232-B4ED-20752F50C8C1}"/>
+  <xr:revisionPtr revIDLastSave="969" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D6F8654-B111-4C5B-B061-C83AE15BEF26}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -598,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -623,7 +623,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,7 +829,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:L42">
-    <sortCondition ref="G4:G42"/>
+    <sortCondition ref="J4:J42"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{9CD2D2FA-51BA-4A30-A0C5-D56FD2E46138}" name="DISCIPLINA" dataDxfId="18"/>
@@ -1159,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,77 +1287,77 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7">
-        <v>3</v>
-      </c>
       <c r="K7" s="2">
-        <v>14472</v>
+        <v>11792</v>
       </c>
       <c r="L7" s="5">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
       <c r="K8" s="2">
-        <v>14472</v>
+        <v>13034</v>
       </c>
       <c r="L8" s="5">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1373,27 +1372,27 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
         <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
-        <v>45000</v>
+        <v>13070</v>
       </c>
       <c r="L9" s="5">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1408,30 +1407,30 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
         <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
-        <v>14616</v>
+        <v>13070</v>
       </c>
       <c r="L10" s="5">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -1443,62 +1442,62 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
         <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K11" s="2">
-        <v>12274</v>
+        <v>11792</v>
       </c>
       <c r="L11" s="5">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
         <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="J12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" s="2">
-        <v>14642</v>
+        <v>45000</v>
       </c>
       <c r="L12" s="5">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1513,33 +1512,33 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H13" t="s">
         <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K13" s="2">
-        <v>14472</v>
+        <v>45000</v>
       </c>
       <c r="L13" s="5">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -1548,68 +1547,68 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H14" t="s">
         <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K14" s="2">
-        <v>13034</v>
+        <v>45000</v>
       </c>
       <c r="L14" s="5">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
       <c r="K15" s="2">
-        <v>12203</v>
+        <v>14472</v>
       </c>
       <c r="L15" s="5">
-        <v>71</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -1618,68 +1617,68 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
         <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K16" s="2">
-        <v>11792</v>
+        <v>14472</v>
       </c>
       <c r="L16" s="5">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="H17" t="s">
         <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K17" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
       <c r="L17" s="5">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -1688,27 +1687,27 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="H18" t="s">
         <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18" s="2">
-        <v>11792</v>
+        <v>14472</v>
       </c>
       <c r="L18" s="5">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1720,33 +1719,33 @@
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
         <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K19" s="2">
-        <v>14875</v>
+        <v>12203</v>
       </c>
       <c r="L19" s="5">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -1755,30 +1754,30 @@
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="H20" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="J20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" s="2">
-        <v>45000</v>
+        <v>14091</v>
       </c>
       <c r="L20" s="5">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -1793,27 +1792,27 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H21" t="s">
         <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K21" s="2">
-        <v>45000</v>
+        <v>13034</v>
       </c>
       <c r="L21" s="5">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -1828,33 +1827,33 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
         <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K22" s="2">
-        <v>13070</v>
+        <v>13034</v>
       </c>
       <c r="L22" s="5">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -1863,27 +1862,27 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
         <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K23" s="2">
-        <v>13070</v>
+        <v>13034</v>
       </c>
       <c r="L23" s="5">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -1898,33 +1897,33 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H24" t="s">
         <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J24">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K24" s="2">
-        <v>14642</v>
+        <v>14091</v>
       </c>
       <c r="L24" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -1933,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H25" t="s">
         <v>73</v>
@@ -1945,18 +1944,18 @@
         <v>4</v>
       </c>
       <c r="K25" s="2">
-        <v>14091</v>
+        <v>14525</v>
       </c>
       <c r="L25" s="5">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -1965,36 +1964,36 @@
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="H26" t="s">
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K26" s="2">
-        <v>14091</v>
+        <v>14642</v>
       </c>
       <c r="L26" s="5">
-        <v>53</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -2003,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
         <v>73</v>
@@ -2015,21 +2014,21 @@
         <v>5</v>
       </c>
       <c r="K27" s="2">
-        <v>14642</v>
+        <v>12274</v>
       </c>
       <c r="L27" s="5">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -2038,27 +2037,27 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="H28" t="s">
         <v>73</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J28">
         <v>5</v>
       </c>
       <c r="K28" s="2">
-        <v>14875</v>
+        <v>14642</v>
       </c>
       <c r="L28" s="5">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
@@ -2073,68 +2072,68 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H29" t="s">
         <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K29" s="2">
-        <v>13000</v>
+        <v>14875</v>
       </c>
       <c r="L29" s="5">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" t="s">
+        <v>81</v>
+      </c>
+      <c r="J30">
         <v>5</v>
       </c>
-      <c r="C30" s="1">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" t="s">
-        <v>73</v>
-      </c>
-      <c r="I30" t="s">
-        <v>76</v>
-      </c>
-      <c r="J30">
-        <v>4</v>
-      </c>
       <c r="K30" s="2">
-        <v>14525</v>
+        <v>13034</v>
       </c>
       <c r="L30" s="5">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C31" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -2143,62 +2142,62 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s">
         <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J31">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K31" s="2">
-        <v>45000</v>
+        <v>14525</v>
       </c>
       <c r="L31" s="5">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" t="s">
+        <v>77</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="K32" s="2">
+        <v>14776</v>
+      </c>
+      <c r="L32" s="5">
         <v>17</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2</v>
-      </c>
-      <c r="D32" s="1">
-        <v>2</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" t="s">
-        <v>58</v>
-      </c>
-      <c r="H32" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" t="s">
-        <v>75</v>
-      </c>
-      <c r="J32">
-        <v>7</v>
-      </c>
-      <c r="K32" s="2">
-        <v>13070</v>
-      </c>
-      <c r="L32" s="5">
-        <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -2213,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H33" t="s">
         <v>73</v>
@@ -2222,24 +2221,24 @@
         <v>80</v>
       </c>
       <c r="J33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K33" s="2">
-        <v>14642</v>
+        <v>45000</v>
       </c>
       <c r="L33" s="5">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -2248,30 +2247,30 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
         <v>73</v>
       </c>
       <c r="I34" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K34" s="2">
-        <v>14642</v>
+        <v>13000</v>
       </c>
       <c r="L34" s="5">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -2283,33 +2282,33 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H35" t="s">
         <v>73</v>
       </c>
       <c r="I35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K35" s="2">
-        <v>13034</v>
+        <v>14525</v>
       </c>
       <c r="L35" s="5">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C36" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
@@ -2318,33 +2317,33 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="H36" t="s">
         <v>73</v>
       </c>
       <c r="I36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J36">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K36" s="2">
-        <v>14525</v>
+        <v>14616</v>
       </c>
       <c r="L36" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C37" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -2353,33 +2352,33 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H37" t="s">
         <v>73</v>
       </c>
       <c r="I37" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J37">
         <v>7</v>
       </c>
       <c r="K37" s="2">
-        <v>13000</v>
+        <v>14875</v>
       </c>
       <c r="L37" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -2388,27 +2387,27 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="H38" t="s">
         <v>73</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J38">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K38" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
       <c r="L38" s="5">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -2423,33 +2422,33 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="H39" t="s">
         <v>73</v>
       </c>
       <c r="I39" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J39">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K39" s="2">
-        <v>13034</v>
+        <v>13070</v>
       </c>
       <c r="L39" s="5">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C40" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -2458,33 +2457,33 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H40" t="s">
         <v>73</v>
       </c>
       <c r="I40" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J40">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K40" s="2">
-        <v>14776</v>
+        <v>13000</v>
       </c>
       <c r="L40" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C41" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -2493,33 +2492,33 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="H41" t="s">
         <v>73</v>
       </c>
       <c r="I41" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K41" s="2">
-        <v>14525</v>
+        <v>11792</v>
       </c>
       <c r="L41" s="5">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -2528,22 +2527,22 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="H42" t="s">
         <v>73</v>
       </c>
       <c r="I42" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J42">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K42" s="2">
-        <v>11792</v>
+        <v>14642</v>
       </c>
       <c r="L42" s="5">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2599,7 +2598,7 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+      <c r="B5" t="s">
         <v>117</v>
       </c>
       <c r="C5" t="s">
@@ -2731,7 +2730,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
+      <c r="B17" t="s">
         <v>117</v>
       </c>
       <c r="C17" t="s">
@@ -2886,7 +2885,7 @@
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="12" t="s">
+      <c r="B31" t="s">
         <v>117</v>
       </c>
       <c r="C31" t="s">
@@ -3007,7 +3006,7 @@
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="12" t="s">
+      <c r="B42" t="s">
         <v>117</v>
       </c>
       <c r="C42" t="s">
@@ -3135,7 +3134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E06C8D-EBEC-4F83-9AB8-8954035C71B9}">
   <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Algorithm works but not so fast
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="969" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D6F8654-B111-4C5B-B061-C83AE15BEF26}"/>
+  <xr:revisionPtr revIDLastSave="970" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBBF72DC-D449-4D0D-ABB4-F42A9E97BE96}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -829,7 +829,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:L42">
-    <sortCondition ref="J4:J42"/>
+    <sortCondition ref="B4:B42"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{9CD2D2FA-51BA-4A30-A0C5-D56FD2E46138}" name="DISCIPLINA" dataDxfId="18"/>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -1232,33 +1232,33 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
         <v>73</v>
       </c>
       <c r="I5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5" s="2">
-        <v>11785</v>
+        <v>45000</v>
       </c>
       <c r="L5" s="5">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -1267,103 +1267,103 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
         <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K6" s="2">
-        <v>11785</v>
+        <v>14091</v>
       </c>
       <c r="L6" s="5">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7">
         <v>4</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
       <c r="K7" s="2">
-        <v>11792</v>
+        <v>13034</v>
       </c>
       <c r="L7" s="5">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
         <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K8" s="2">
-        <v>13034</v>
+        <v>14525</v>
       </c>
       <c r="L8" s="5">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -1372,33 +1372,33 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="H9" t="s">
         <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K9" s="2">
-        <v>13070</v>
+        <v>14642</v>
       </c>
       <c r="L9" s="5">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -1407,33 +1407,33 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
         <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K10" s="2">
-        <v>13070</v>
+        <v>12274</v>
       </c>
       <c r="L10" s="5">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -1442,30 +1442,30 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>128</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
         <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K11" s="2">
-        <v>11792</v>
+        <v>14875</v>
       </c>
       <c r="L11" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -1474,30 +1474,30 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
         <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K12" s="2">
-        <v>45000</v>
+        <v>14525</v>
       </c>
       <c r="L12" s="5">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1512,16 +1512,16 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
         <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K13" s="2">
         <v>45000</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1547,30 +1547,30 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
         <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K14" s="2">
-        <v>45000</v>
+        <v>13000</v>
       </c>
       <c r="L14" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1582,33 +1582,33 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K15" s="2">
-        <v>14472</v>
+        <v>14525</v>
       </c>
       <c r="L15" s="5">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -1617,33 +1617,33 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
         <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K16" s="2">
-        <v>14472</v>
+        <v>14642</v>
       </c>
       <c r="L16" s="5">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -1652,27 +1652,27 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
         <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K17" s="2">
-        <v>14642</v>
+        <v>14875</v>
       </c>
       <c r="L17" s="5">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -1687,97 +1687,97 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="H18" t="s">
         <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K18" s="2">
-        <v>14472</v>
+        <v>14616</v>
       </c>
       <c r="L18" s="5">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H19" t="s">
         <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K19" s="2">
-        <v>12203</v>
+        <v>13000</v>
       </c>
       <c r="L19" s="5">
-        <v>71</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="H20" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K20" s="2">
-        <v>14091</v>
+        <v>13070</v>
       </c>
       <c r="L20" s="5">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -1792,42 +1792,42 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H21" t="s">
         <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J21">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K21" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
       <c r="L21" s="5">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="H22" t="s">
         <v>73</v>
@@ -1839,30 +1839,30 @@
         <v>3</v>
       </c>
       <c r="K22" s="2">
-        <v>13034</v>
+        <v>14091</v>
       </c>
       <c r="L22" s="5">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
       <c r="G23" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="H23" t="s">
         <v>73</v>
@@ -1871,24 +1871,24 @@
         <v>76</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K23" s="2">
-        <v>13034</v>
+        <v>45000</v>
       </c>
       <c r="L23" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -1897,68 +1897,68 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="H24" t="s">
         <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K24" s="2">
-        <v>14091</v>
+        <v>45000</v>
       </c>
       <c r="L24" s="5">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
         <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="J25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K25" s="2">
-        <v>14525</v>
+        <v>12203</v>
       </c>
       <c r="L25" s="5">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -1967,33 +1967,33 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H26" t="s">
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K26" s="2">
-        <v>14642</v>
+        <v>14472</v>
       </c>
       <c r="L26" s="5">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -2002,33 +2002,33 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H27" t="s">
         <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K27" s="2">
-        <v>12274</v>
+        <v>14472</v>
       </c>
       <c r="L27" s="5">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="H28" t="s">
         <v>73</v>
@@ -2049,21 +2049,21 @@
         <v>5</v>
       </c>
       <c r="K28" s="2">
-        <v>14642</v>
+        <v>14776</v>
       </c>
       <c r="L28" s="5">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -2072,33 +2072,33 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="H29" t="s">
         <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J29">
         <v>5</v>
       </c>
       <c r="K29" s="2">
-        <v>14875</v>
+        <v>13034</v>
       </c>
       <c r="L29" s="5">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C30" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -2107,33 +2107,33 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
       <c r="H30" t="s">
         <v>73</v>
       </c>
       <c r="I30" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="J30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K30" s="2">
-        <v>13034</v>
+        <v>11792</v>
       </c>
       <c r="L30" s="5">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C31" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -2142,33 +2142,33 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="H31" t="s">
         <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="J31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K31" s="2">
-        <v>14525</v>
+        <v>13070</v>
       </c>
       <c r="L31" s="5">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -2177,27 +2177,27 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H32" t="s">
         <v>73</v>
       </c>
       <c r="I32" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="J32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K32" s="2">
-        <v>14776</v>
+        <v>13070</v>
       </c>
       <c r="L32" s="5">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -2212,27 +2212,27 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="H33" t="s">
         <v>73</v>
       </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="J33">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K33" s="2">
-        <v>45000</v>
+        <v>11785</v>
       </c>
       <c r="L33" s="5">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -2247,103 +2247,103 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H34" t="s">
         <v>73</v>
       </c>
       <c r="I34" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="J34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K34" s="2">
-        <v>13000</v>
+        <v>11785</v>
       </c>
       <c r="L34" s="5">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35">
         <v>1</v>
       </c>
-      <c r="D35" s="1">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-      <c r="G35" t="s">
-        <v>54</v>
-      </c>
-      <c r="H35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" t="s">
-        <v>82</v>
-      </c>
-      <c r="J35">
-        <v>6</v>
-      </c>
       <c r="K35" s="2">
-        <v>14525</v>
+        <v>11792</v>
       </c>
       <c r="L35" s="5">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="H36" t="s">
         <v>73</v>
       </c>
       <c r="I36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J36">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K36" s="2">
-        <v>14616</v>
+        <v>13034</v>
       </c>
       <c r="L36" s="5">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -2352,33 +2352,33 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="H37" t="s">
         <v>73</v>
       </c>
       <c r="I37" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J37">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K37" s="2">
-        <v>14875</v>
+        <v>13034</v>
       </c>
       <c r="L37" s="5">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -2387,27 +2387,27 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="H38" t="s">
         <v>73</v>
       </c>
       <c r="I38" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J38">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K38" s="2">
-        <v>14642</v>
+        <v>13034</v>
       </c>
       <c r="L38" s="5">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -2422,62 +2422,62 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="H39" t="s">
         <v>73</v>
       </c>
       <c r="I39" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J39">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K39" s="2">
-        <v>13070</v>
+        <v>14642</v>
       </c>
       <c r="L39" s="5">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>70</v>
+      </c>
+      <c r="H40" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" t="s">
+        <v>83</v>
+      </c>
+      <c r="J40">
         <v>3</v>
       </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>57</v>
-      </c>
-      <c r="H40" t="s">
-        <v>73</v>
-      </c>
-      <c r="I40" t="s">
-        <v>78</v>
-      </c>
-      <c r="J40">
-        <v>7</v>
-      </c>
       <c r="K40" s="2">
-        <v>13000</v>
+        <v>14472</v>
       </c>
       <c r="L40" s="5">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
@@ -2492,33 +2492,33 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H41" t="s">
         <v>73</v>
       </c>
       <c r="I41" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J41">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K41" s="2">
         <v>11792</v>
       </c>
       <c r="L41" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C42" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -2527,22 +2527,22 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="H42" t="s">
         <v>73</v>
       </c>
       <c r="I42" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="J42">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K42" s="2">
         <v>14642</v>
       </c>
       <c r="L42" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2561,7 +2561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177CF1B3-023B-4C26-8BA7-3BF936A39EC1}">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Starting with numpy and OOP implementation
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1027" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B89DECD0-49EE-4370-8F15-0FC4222D7BE3}"/>
+  <xr:revisionPtr revIDLastSave="1029" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{580C9C2B-E76F-4154-9757-C32ED7FEAA25}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,6 +1040,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
@@ -1090,7 +1094,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}" name="Table167" displayName="Table167" ref="A1:K34" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:K34" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K34">
-    <sortCondition ref="I1:I34"/>
+    <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{99E45A2F-9332-4CFA-9CF0-E4A298DC69DF}" name="DISCIPLINA" dataDxfId="18"/>
@@ -1113,7 +1117,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}" name="Table2" displayName="Table2" ref="B4:D51" totalsRowShown="0">
   <autoFilter ref="B4:D51" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:D51">
-    <sortCondition ref="D4:D51"/>
+    <sortCondition ref="B4:B51"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DA2ECD09-3FA6-4544-AE27-6E4A1304C0F4}" name="DISCIPLINA"/>
@@ -4013,8 +4017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C694DF4-CEA0-4BF6-94BA-E896B085E534}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4056,7 +4060,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -4071,33 +4075,33 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
         <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" s="2">
-        <v>13070</v>
+        <v>45000</v>
       </c>
       <c r="K2" s="5">
-        <v>61</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -4106,103 +4110,103 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
         <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J3" s="2">
-        <v>11785</v>
+        <v>14091</v>
       </c>
       <c r="K3" s="5">
-        <v>56</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4" s="2">
-        <v>11792</v>
+        <v>13034</v>
       </c>
       <c r="K4" s="5">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
         <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J5" s="2">
-        <v>13034</v>
+        <v>14525</v>
       </c>
       <c r="K5" s="5">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -4211,30 +4215,30 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
         <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J6" s="2">
-        <v>45000</v>
+        <v>14642</v>
       </c>
       <c r="K6" s="5">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -4243,30 +4247,30 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
         <v>73</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J7" s="2">
-        <v>45000</v>
+        <v>12274</v>
       </c>
       <c r="K7" s="5">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -4281,27 +4285,27 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J8" s="2">
-        <v>45000</v>
+        <v>14875</v>
       </c>
       <c r="K8" s="5">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -4316,100 +4320,100 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J9" s="2">
-        <v>11792</v>
+        <v>14525</v>
       </c>
       <c r="K9" s="5">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s">
         <v>73</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J10" s="2">
-        <v>14091</v>
+        <v>45000</v>
       </c>
       <c r="K10" s="5">
-        <v>53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J11" s="2">
-        <v>12203</v>
+        <v>13000</v>
       </c>
       <c r="K11" s="5">
-        <v>71</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -4421,33 +4425,33 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J12" s="2">
-        <v>14472</v>
+        <v>14525</v>
       </c>
       <c r="K12" s="5">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -4456,33 +4460,33 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
         <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J13" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
       <c r="K13" s="5">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -4491,33 +4495,33 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
         <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J14" s="2">
-        <v>14472</v>
+        <v>14875</v>
       </c>
       <c r="K14" s="5">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -4526,30 +4530,30 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="G15" t="s">
         <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J15" s="2">
-        <v>14091</v>
+        <v>14616</v>
       </c>
       <c r="K15" s="5">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -4561,27 +4565,27 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G16" t="s">
         <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J16" s="2">
-        <v>13034</v>
+        <v>13000</v>
       </c>
       <c r="K16" s="5">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -4596,33 +4600,33 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G17" t="s">
         <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J17" s="2">
-        <v>14525</v>
+        <v>13070</v>
       </c>
       <c r="K17" s="5">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -4631,65 +4635,65 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
         <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J18" s="2">
         <v>14642</v>
       </c>
       <c r="K18" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19">
         <v>3</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19">
-        <v>5</v>
-      </c>
       <c r="J19" s="2">
-        <v>14642</v>
+        <v>14091</v>
       </c>
       <c r="K19" s="5">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -4698,30 +4702,30 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
         <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J20" s="2">
-        <v>12274</v>
+        <v>45000</v>
       </c>
       <c r="K20" s="5">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -4736,30 +4740,30 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
         <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J21" s="2">
-        <v>14875</v>
+        <v>45000</v>
       </c>
       <c r="K21" s="5">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -4768,36 +4772,36 @@
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
         <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J22" s="2">
-        <v>14525</v>
+        <v>12203</v>
       </c>
       <c r="K22" s="5">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -4806,33 +4810,33 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" t="s">
         <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J23" s="2">
-        <v>14776</v>
+        <v>14472</v>
       </c>
       <c r="K23" s="5">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -4841,33 +4845,33 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
         <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I24">
         <v>5</v>
       </c>
       <c r="J24" s="2">
-        <v>13034</v>
+        <v>14776</v>
       </c>
       <c r="K24" s="5">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -4876,33 +4880,33 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="G25" t="s">
         <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J25" s="2">
-        <v>45000</v>
+        <v>13034</v>
       </c>
       <c r="K25" s="5">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B26" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -4911,68 +4915,68 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="G26" t="s">
         <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J26" s="2">
-        <v>13000</v>
+        <v>11792</v>
       </c>
       <c r="K26" s="5">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I27">
         <v>1</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" t="s">
-        <v>82</v>
-      </c>
-      <c r="I27">
-        <v>6</v>
-      </c>
       <c r="J27" s="2">
-        <v>14525</v>
+        <v>13070</v>
       </c>
       <c r="K27" s="5">
-        <v>4</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -4981,30 +4985,30 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="G28" t="s">
         <v>73</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I28">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J28" s="2">
-        <v>14642</v>
+        <v>11785</v>
       </c>
       <c r="K28" s="5">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -5016,97 +5020,97 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="G29" t="s">
         <v>73</v>
       </c>
       <c r="H29" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J29" s="2">
-        <v>14875</v>
+        <v>11792</v>
       </c>
       <c r="K29" s="5">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="G30" t="s">
         <v>73</v>
       </c>
       <c r="H30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I30">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J30" s="2">
-        <v>14616</v>
+        <v>13034</v>
       </c>
       <c r="K30" s="5">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31">
         <v>3</v>
       </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31">
-        <v>7</v>
-      </c>
       <c r="J31" s="2">
-        <v>13000</v>
+        <v>13034</v>
       </c>
       <c r="K31" s="5">
-        <v>19</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="B32" s="1">
         <v>2</v>
@@ -5121,27 +5125,27 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
         <v>73</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J32" s="2">
-        <v>13070</v>
+        <v>14472</v>
       </c>
       <c r="K32" s="5">
-        <v>14</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
@@ -5156,33 +5160,33 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G33" t="s">
         <v>73</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I33">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J33" s="2">
         <v>11792</v>
       </c>
       <c r="K33" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -5191,22 +5195,22 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G34" t="s">
         <v>73</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="I34">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J34" s="2">
         <v>14642</v>
       </c>
       <c r="K34" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -5221,8 +5225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177CF1B3-023B-4C26-8BA7-3BF936A39EC1}">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5259,76 +5263,76 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2">
-        <v>11785</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2">
-        <v>11792</v>
+        <v>14091</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2">
-        <v>11792</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2">
-        <v>11792</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2">
-        <v>12203</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="D10" s="2">
-        <v>12274</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D11" s="2">
         <v>12274</v>
@@ -5336,43 +5340,43 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D12" s="2">
-        <v>12274</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2">
-        <v>13000</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2">
-        <v>13000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2">
         <v>13000</v>
@@ -5380,76 +5384,76 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2">
-        <v>13000</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2">
-        <v>13034</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D19" s="2">
-        <v>13034</v>
+        <v>14616</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2">
-        <v>13034</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2">
-        <v>13034</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2">
         <v>13070</v>
@@ -5457,24 +5461,24 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2">
-        <v>13070</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D24" s="2">
-        <v>14091</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
@@ -5490,44 +5494,44 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D26" s="2">
-        <v>14472</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D27" s="2">
-        <v>14472</v>
+        <v>45000</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D28" s="2">
-        <v>14472</v>
+        <v>12203</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" s="2">
         <v>14472</v>
@@ -5535,244 +5539,244 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D30" s="2">
-        <v>14472</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D31" s="2">
-        <v>14525</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="D32" s="2">
-        <v>14525</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D33" s="2">
-        <v>14525</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2">
-        <v>14525</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="D35" s="2">
-        <v>14616</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="D36" s="2">
-        <v>14642</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D37" s="2">
-        <v>14642</v>
+        <v>13070</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D38" s="2">
-        <v>14642</v>
+        <v>11785</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="D39" s="2">
-        <v>14642</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D40" s="2">
-        <v>14642</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D41" s="2">
-        <v>14642</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="D42" s="2">
-        <v>14776</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="D43" s="2">
-        <v>14776</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="D44" s="2">
-        <v>14776</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D45" s="2">
-        <v>14875</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D46" s="2">
-        <v>14875</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D47" s="2">
-        <v>14875</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D48" s="2">
-        <v>45000</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D49" s="2">
-        <v>45000</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="D50" s="2">
-        <v>45000</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D51" s="2">
-        <v>45000</v>
+        <v>14642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost ready making use of np arrays
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1029" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{580C9C2B-E76F-4154-9757-C32ED7FEAA25}"/>
+  <xr:revisionPtr revIDLastSave="1035" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89E3E9E4-C58C-4D32-9949-F7FE0C3A1398}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="150">
   <si>
     <t>CURSO: ENGENHARIA DE SOFTWARE</t>
   </si>
@@ -628,7 +628,120 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="61">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1040,74 +1153,70 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:L42">
     <sortCondition ref="B4:B42"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{9CD2D2FA-51BA-4A30-A0C5-D56FD2E46138}" name="DISCIPLINA" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{2A5DB422-BF96-43DC-A9BA-12634A4F2BBC}" name="AT" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{EE047B0A-B831-48AA-B73B-E1927AF8CC86}" name="AP" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{C513E1E7-AAE7-4E76-9F05-8997EF765B3F}" name="AE" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{C8FF95F3-B743-4CF1-BB31-5218A0DEB0E2}" name="AV" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{E65FE900-9015-483F-BD63-03E8F53E8070}" name="NOME" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{83B8989C-17F6-4ED6-98C3-45E8D442FFE7}" name="CR" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{027923F2-5900-43B1-A215-2A9BC846F14C}" name="SL/B" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{DF7BF826-9991-4443-82C2-9826A1B4EDBC}" name="ET" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{D1A1A381-59C2-4080-BEF8-40B8E70D1796}" name="PROFESSOR" dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{ADC459DE-BDC9-454A-824A-24BCD3A9031B}" name="ALUNOS MATRIC" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{9CD2D2FA-51BA-4A30-A0C5-D56FD2E46138}" name="DISCIPLINA" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{2A5DB422-BF96-43DC-A9BA-12634A4F2BBC}" name="AT" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{EE047B0A-B831-48AA-B73B-E1927AF8CC86}" name="AP" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{C513E1E7-AAE7-4E76-9F05-8997EF765B3F}" name="AE" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{C8FF95F3-B743-4CF1-BB31-5218A0DEB0E2}" name="AV" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{E65FE900-9015-483F-BD63-03E8F53E8070}" name="NOME" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{83B8989C-17F6-4ED6-98C3-45E8D442FFE7}" name="CR" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{027923F2-5900-43B1-A215-2A9BC846F14C}" name="SL/B" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{DF7BF826-9991-4443-82C2-9826A1B4EDBC}" name="ET" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{D1A1A381-59C2-4080-BEF8-40B8E70D1796}" name="PROFESSOR" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{ADC459DE-BDC9-454A-824A-24BCD3A9031B}" name="ALUNOS MATRIC" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{94BB9D13-CA19-4CA7-94BE-33C56E1E2F75}" name="Table16" displayName="Table16" ref="B44:L77" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{94BB9D13-CA19-4CA7-94BE-33C56E1E2F75}" name="Table16" displayName="Table16" ref="B44:L77" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="B44:L77" xr:uid="{94BB9D13-CA19-4CA7-94BE-33C56E1E2F75}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B45:L77">
     <sortCondition ref="B4:B42"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{706AB578-0B6F-43D3-BB61-D3E63C94C5C5}" name="DISCIPLINA" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{92C94A86-2FEF-421A-9CC5-CA7D417108D9}" name="AT" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{9907E328-02FC-4373-9361-D2E3BFE226DC}" name="AP" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{A7CC33C0-52CA-4582-8FF1-FEFEAE72EB0E}" name="AE" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{D8AFF64B-A3E3-413C-849B-0F0D3870941F}" name="AV" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{0CF01315-BEA4-4A80-9E81-286A7F94C7FA}" name="NOME" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{609DFCD0-358B-4053-86D5-D40C402E2F98}" name="CR" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{CD3E01FB-E340-4977-B45E-4E889CC1EAFA}" name="SL/B" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{6673106B-E091-46CB-9070-C0EE46C9E65E}" name="ET" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{26E42379-0ED6-41FA-A822-65DF2989814F}" name="PROFESSOR" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{1D04ED35-AD87-4382-977E-E166AC54C0B0}" name="ALUNOS MATRIC" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{706AB578-0B6F-43D3-BB61-D3E63C94C5C5}" name="DISCIPLINA" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{92C94A86-2FEF-421A-9CC5-CA7D417108D9}" name="AT" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{9907E328-02FC-4373-9361-D2E3BFE226DC}" name="AP" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{A7CC33C0-52CA-4582-8FF1-FEFEAE72EB0E}" name="AE" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{D8AFF64B-A3E3-413C-849B-0F0D3870941F}" name="AV" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{0CF01315-BEA4-4A80-9E81-286A7F94C7FA}" name="NOME" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{609DFCD0-358B-4053-86D5-D40C402E2F98}" name="CR" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{CD3E01FB-E340-4977-B45E-4E889CC1EAFA}" name="SL/B" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{6673106B-E091-46CB-9070-C0EE46C9E65E}" name="ET" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{26E42379-0ED6-41FA-A822-65DF2989814F}" name="PROFESSOR" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{1D04ED35-AD87-4382-977E-E166AC54C0B0}" name="ALUNOS MATRIC" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}" name="Table167" displayName="Table167" ref="A1:K34" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}" name="Table167" displayName="Table167" ref="A1:K34" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A1:K34" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K34">
     <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{99E45A2F-9332-4CFA-9CF0-E4A298DC69DF}" name="DISCIPLINA" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{4173FD76-8105-47F9-9DCE-D3B021A0F29D}" name="AT" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{8F80F768-1203-466E-B79F-E0C4F4AFAAB8}" name="AP" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{78918C4C-9168-4FAB-A2E3-24E3F8D870F8}" name="AE" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{B5F37458-7439-4148-8012-8EB48E3DD8D0}" name="AV" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{6F7EA491-05CE-4E0D-8968-65BA2793D6E8}" name="NOME" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{20008DE3-D13C-44CF-8CAA-58EC6DDABBBC}" name="CR" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{6789E295-1ACD-4B11-A4F9-01F3CECC14FA}" name="SL/B" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{509CA827-6B56-4C16-9CB0-D43DB4AF1E43}" name="ET" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{CC966D57-ACED-4B16-9CB1-406220269B5E}" name="PROFESSOR" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{20302694-742B-4E98-81D5-F6BA62536451}" name="ALUNOS MATRIC" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{99E45A2F-9332-4CFA-9CF0-E4A298DC69DF}" name="DISCIPLINA" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{4173FD76-8105-47F9-9DCE-D3B021A0F29D}" name="AT" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{8F80F768-1203-466E-B79F-E0C4F4AFAAB8}" name="AP" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{78918C4C-9168-4FAB-A2E3-24E3F8D870F8}" name="AE" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{B5F37458-7439-4148-8012-8EB48E3DD8D0}" name="AV" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{6F7EA491-05CE-4E0D-8968-65BA2793D6E8}" name="NOME" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{20008DE3-D13C-44CF-8CAA-58EC6DDABBBC}" name="CR" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{6789E295-1ACD-4B11-A4F9-01F3CECC14FA}" name="SL/B" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{509CA827-6B56-4C16-9CB0-D43DB4AF1E43}" name="ET" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{CC966D57-ACED-4B16-9CB1-406220269B5E}" name="PROFESSOR" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{20302694-742B-4E98-81D5-F6BA62536451}" name="ALUNOS MATRIC" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1122,7 +1231,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DA2ECD09-3FA6-4544-AE27-6E4A1304C0F4}" name="DISCIPLINA"/>
     <tableColumn id="2" xr3:uid="{C1D61556-D79E-4B3D-AE1A-582127EF40D7}" name="NOME"/>
-    <tableColumn id="3" xr3:uid="{0169D052-F3EC-453E-B9FA-D7EB40423470}" name="PROFESSOR CODE" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0169D052-F3EC-453E-B9FA-D7EB40423470}" name="PROFESSOR CODE" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1135,7 +1244,7 @@
     <sortCondition ref="B4:B19"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BAE49131-A56E-44EB-BD41-330691452D20}" name="CODE" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{BAE49131-A56E-44EB-BD41-330691452D20}" name="CODE" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{EC56BC82-9C5A-473A-9BF8-799826212E29}" name="NOME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1143,18 +1252,55 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}" name="Table4" displayName="Table4" ref="I2:L35" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}" name="Table4" displayName="Table4" ref="I2:L35" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="I2:L35" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:L35">
     <sortCondition ref="L2:L35"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C8A0A278-3838-4995-8588-B07D13EA3EFD}" name="NOME" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{D7D84DAB-D2AE-4879-9CEE-32E7CA42BC4C}" name="CR" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{60337C39-789F-4651-A8AB-E68BD1E538E3}" name="SL/B" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{4DEB40D6-B26B-4C55-8BD0-3BE4E24E00B0}" name="ET" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C8A0A278-3838-4995-8588-B07D13EA3EFD}" name="NOME" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{D7D84DAB-D2AE-4879-9CEE-32E7CA42BC4C}" name="CR" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{60337C39-789F-4651-A8AB-E68BD1E538E3}" name="SL/B" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{4DEB40D6-B26B-4C55-8BD0-3BE4E24E00B0}" name="ET" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{481FA10C-0BC0-4E91-B80D-8591478485CF}" name="Table18" displayName="Table18" ref="B38:L53" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="B38:L53" xr:uid="{481FA10C-0BC0-4E91-B80D-8591478485CF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B39:L53">
+    <sortCondition ref="K38:K53"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{F372217B-2A68-4004-9285-10D7E90A0B0E}" name="DISCIPLINA" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C3BB104A-81EF-4C52-A9A7-530A07856212}" name="AT" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{9B4C9EEB-F5DD-482F-95C3-C29CAEFFAC7E}" name="AP" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{96A7B98D-1D2D-44E9-8260-91F05512BE0F}" name="AE" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{D4B47FCE-9802-417E-9CFB-9D6A58D0BACD}" name="AV" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{F9B14BF4-A785-46B9-A7D3-7B536EE599CC}" name="NOME" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1E7008A2-4E60-4A02-A858-067C78FF6A22}" name="CR" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{667FADCE-6DFF-44D9-AB54-CD21B2BDF7F0}" name="SL/B" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{2D307CC2-649E-4D1E-91FA-80EE15A24E37}" name="ET" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{E92D9F71-5E60-4BCC-A870-768E44959260}" name="PROFESSOR" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{BF05BD94-4998-4F11-8493-3B000AE8928B}" name="ALUNOS MATRIC" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C94CF6EC-5DC4-4F85-9B0C-70D8A6D701D3}" name="Table39" displayName="Table39" ref="N38:O53" totalsRowShown="0">
+  <autoFilter ref="N38:O53" xr:uid="{C94CF6EC-5DC4-4F85-9B0C-70D8A6D701D3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N39:O53">
+    <sortCondition ref="N4:N19"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F31A5C4C-7274-4461-9C86-51126542426E}" name="CODE" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{FBEE49C1-B9C9-4BCA-8857-9A5002D2147E}" name="NOME"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1423,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L77"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:L77"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4017,7 +4163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C694DF4-CEA0-4BF6-94BA-E896B085E534}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5799,7 +5945,7 @@
   <dimension ref="B1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5977,10 +6123,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71808F-48CA-4498-917A-4D75806DE602}">
-  <dimension ref="B2:L35"/>
+  <dimension ref="B2:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6515,7 +6661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>65</v>
       </c>
@@ -6532,7 +6678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
         <v>54</v>
       </c>
@@ -6549,7 +6695,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>129</v>
       </c>
@@ -6566,10 +6712,668 @@
         <v>8</v>
       </c>
     </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" t="s">
+        <v>72</v>
+      </c>
+      <c r="I38" t="s">
+        <v>74</v>
+      </c>
+      <c r="J38" t="s">
+        <v>88</v>
+      </c>
+      <c r="K38" t="s">
+        <v>89</v>
+      </c>
+      <c r="L38" t="s">
+        <v>105</v>
+      </c>
+      <c r="N38" t="s">
+        <v>144</v>
+      </c>
+      <c r="O38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" t="s">
+        <v>86</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>11785</v>
+      </c>
+      <c r="L39" s="5">
+        <v>26</v>
+      </c>
+      <c r="N39" s="4">
+        <v>11785</v>
+      </c>
+      <c r="O39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>129</v>
+      </c>
+      <c r="H40" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" t="s">
+        <v>85</v>
+      </c>
+      <c r="J40">
+        <v>7</v>
+      </c>
+      <c r="K40" s="2">
+        <v>11792</v>
+      </c>
+      <c r="L40" s="5">
+        <v>22</v>
+      </c>
+      <c r="N40" s="4">
+        <v>11792</v>
+      </c>
+      <c r="O40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>84</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41" s="2">
+        <v>12203</v>
+      </c>
+      <c r="L41" s="5">
+        <v>71</v>
+      </c>
+      <c r="N41" s="4">
+        <v>12203</v>
+      </c>
+      <c r="O41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42" t="s">
+        <v>73</v>
+      </c>
+      <c r="I42" t="s">
+        <v>77</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+      <c r="K42" s="2">
+        <v>12274</v>
+      </c>
+      <c r="L42" s="5">
+        <v>27</v>
+      </c>
+      <c r="N42" s="4">
+        <v>12274</v>
+      </c>
+      <c r="O42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" t="s">
+        <v>81</v>
+      </c>
+      <c r="J43">
+        <v>6</v>
+      </c>
+      <c r="K43" s="2">
+        <v>13000</v>
+      </c>
+      <c r="L43" s="5">
+        <v>6</v>
+      </c>
+      <c r="N43" s="4">
+        <v>13000</v>
+      </c>
+      <c r="O43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" t="s">
+        <v>73</v>
+      </c>
+      <c r="I44" t="s">
+        <v>76</v>
+      </c>
+      <c r="J44">
+        <v>4</v>
+      </c>
+      <c r="K44" s="2">
+        <v>13034</v>
+      </c>
+      <c r="L44" s="5">
+        <v>11</v>
+      </c>
+      <c r="N44" s="4">
+        <v>13034</v>
+      </c>
+      <c r="O44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H45" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" t="s">
+        <v>75</v>
+      </c>
+      <c r="J45">
+        <v>7</v>
+      </c>
+      <c r="K45" s="2">
+        <v>13070</v>
+      </c>
+      <c r="L45" s="5">
+        <v>14</v>
+      </c>
+      <c r="N45" s="4">
+        <v>13070</v>
+      </c>
+      <c r="O45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>46</v>
+      </c>
+      <c r="H46" t="s">
+        <v>73</v>
+      </c>
+      <c r="I46" t="s">
+        <v>76</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+      <c r="K46" s="2">
+        <v>14091</v>
+      </c>
+      <c r="L46" s="5">
+        <v>14</v>
+      </c>
+      <c r="N46" s="4">
+        <v>14091</v>
+      </c>
+      <c r="O46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" t="s">
+        <v>73</v>
+      </c>
+      <c r="I47" t="s">
+        <v>79</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47" s="2">
+        <v>14472</v>
+      </c>
+      <c r="L47" s="5">
+        <v>28</v>
+      </c>
+      <c r="N47" s="4">
+        <v>14472</v>
+      </c>
+      <c r="O47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" t="s">
+        <v>76</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="K48" s="2">
+        <v>14525</v>
+      </c>
+      <c r="L48" s="5">
+        <v>10</v>
+      </c>
+      <c r="N48" s="4">
+        <v>14525</v>
+      </c>
+      <c r="O48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>108</v>
+      </c>
+      <c r="H49" t="s">
+        <v>73</v>
+      </c>
+      <c r="I49" t="s">
+        <v>80</v>
+      </c>
+      <c r="J49">
+        <v>7</v>
+      </c>
+      <c r="K49" s="2">
+        <v>14616</v>
+      </c>
+      <c r="L49" s="5">
+        <v>22</v>
+      </c>
+      <c r="N49" s="4">
+        <v>14616</v>
+      </c>
+      <c r="O49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I50" t="s">
+        <v>77</v>
+      </c>
+      <c r="J50">
+        <v>5</v>
+      </c>
+      <c r="K50" s="2">
+        <v>14642</v>
+      </c>
+      <c r="L50" s="5">
+        <v>20</v>
+      </c>
+      <c r="N50" s="4">
+        <v>14642</v>
+      </c>
+      <c r="O50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>65</v>
+      </c>
+      <c r="H51" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" t="s">
+        <v>77</v>
+      </c>
+      <c r="J51">
+        <v>5</v>
+      </c>
+      <c r="K51" s="2">
+        <v>14776</v>
+      </c>
+      <c r="L51" s="5">
+        <v>17</v>
+      </c>
+      <c r="N51" s="4">
+        <v>14776</v>
+      </c>
+      <c r="O51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" t="s">
+        <v>73</v>
+      </c>
+      <c r="I52" t="s">
+        <v>78</v>
+      </c>
+      <c r="J52">
+        <v>5</v>
+      </c>
+      <c r="K52" s="2">
+        <v>14875</v>
+      </c>
+      <c r="L52" s="5">
+        <v>16</v>
+      </c>
+      <c r="N52" s="4">
+        <v>14875</v>
+      </c>
+      <c r="O52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s">
+        <v>45</v>
+      </c>
+      <c r="H53" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" t="s">
+        <v>75</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53" s="2">
+        <v>45000</v>
+      </c>
+      <c r="L53" s="5">
+        <v>2</v>
+      </c>
+      <c r="N53" s="4">
+        <v>45000</v>
+      </c>
+      <c r="O53" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OOP works fast with numpy and guided mutation
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1035" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89E3E9E4-C58C-4D32-9949-F7FE0C3A1398}"/>
+  <xr:revisionPtr revIDLastSave="1036" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C900B62-A945-410A-9779-A2AA5386A8E3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -1153,6 +1153,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
@@ -1226,7 +1230,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}" name="Table2" displayName="Table2" ref="B4:D51" totalsRowShown="0">
   <autoFilter ref="B4:D51" xr:uid="{C1443256-B15F-43B7-A450-293B44673D7D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:D51">
-    <sortCondition ref="B4:B51"/>
+    <sortCondition ref="D4:D51"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DA2ECD09-3FA6-4544-AE27-6E4A1304C0F4}" name="DISCIPLINA"/>
@@ -5371,8 +5375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177CF1B3-023B-4C26-8BA7-3BF936A39EC1}">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5409,76 +5413,76 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2">
-        <v>45000</v>
+        <v>11785</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="D6" s="2">
-        <v>14091</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
       <c r="D7" s="2">
-        <v>13034</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="D8" s="2">
-        <v>14472</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2">
-        <v>14525</v>
+        <v>12203</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2">
-        <v>14642</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2">
         <v>12274</v>
@@ -5486,43 +5490,43 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2">
-        <v>14875</v>
+        <v>12274</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2">
-        <v>14525</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2">
-        <v>45000</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2">
         <v>13000</v>
@@ -5530,68 +5534,68 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="D16" s="2">
-        <v>14525</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D17" s="2">
-        <v>14642</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D18" s="2">
-        <v>14875</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2">
-        <v>14616</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="D20" s="2">
-        <v>13000</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D21" s="2">
-        <v>12274</v>
+        <v>13034</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
@@ -5607,24 +5611,24 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D23" s="2">
-        <v>12274</v>
+        <v>13070</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2">
-        <v>14642</v>
+        <v>14091</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
@@ -5640,44 +5644,44 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D26" s="2">
-        <v>45000</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D27" s="2">
-        <v>45000</v>
+        <v>14472</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D28" s="2">
-        <v>12203</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D29" s="2">
         <v>14472</v>
@@ -5685,189 +5689,189 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D30" s="2">
-        <v>14642</v>
+        <v>14472</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D31" s="2">
-        <v>14776</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D32" s="2">
-        <v>13000</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D33" s="2">
-        <v>14776</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D34" s="2">
-        <v>13034</v>
+        <v>14525</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="D35" s="2">
-        <v>14472</v>
+        <v>14616</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D36" s="2">
-        <v>11792</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D37" s="2">
-        <v>13070</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D38" s="2">
-        <v>11785</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D39" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D40" s="2">
-        <v>14525</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D41" s="2">
-        <v>14776</v>
+        <v>14642</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="D42" s="2">
-        <v>11792</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C43" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="D43" s="2">
-        <v>13000</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="D44" s="2">
-        <v>13034</v>
+        <v>14776</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D45" s="2">
-        <v>13034</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D46" s="2">
-        <v>14472</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
@@ -5878,51 +5882,51 @@
         <v>70</v>
       </c>
       <c r="D47" s="2">
-        <v>14472</v>
+        <v>14875</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="D48" s="2">
-        <v>14642</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D49" s="2">
-        <v>14875</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="D50" s="2">
-        <v>11792</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D51" s="2">
-        <v>14642</v>
+        <v>45000</v>
       </c>
     </row>
   </sheetData>
@@ -5945,7 +5949,7 @@
   <dimension ref="B1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C19"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6125,7 +6129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71808F-48CA-4498-917A-4D75806DE602}">
   <dimension ref="B2:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Trying to figure out correct nr of classes
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1036" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C900B62-A945-410A-9779-A2AA5386A8E3}"/>
+  <xr:revisionPtr revIDLastSave="1060" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52FA3F25-4528-4BB5-B4FF-E16F9AD3E979}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="151">
   <si>
     <t>CURSO: ENGENHARIA DE SOFTWARE</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>AB122</t>
+  </si>
+  <si>
+    <t>Hours</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,24 +532,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor theme="6" tint="0.59999389629810485"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor theme="6" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor theme="7"/>
       </patternFill>
     </fill>
   </fills>
@@ -599,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -612,9 +597,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,14 +606,129 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="67">
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -739,70 +836,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.79998168889431442"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.79998168889431442"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.79998168889431442"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.79998168889431442"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.79998168889431442"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="7"/>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1158,69 +1191,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}" name="Table1" displayName="Table1" ref="B4:L42" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="B4:L42" xr:uid="{00E4B722-195D-4DBA-ABF6-2A9F8F42EDB9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:L42">
-    <sortCondition ref="B4:B42"/>
+    <sortCondition ref="J4:J42"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{9CD2D2FA-51BA-4A30-A0C5-D56FD2E46138}" name="DISCIPLINA" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{2A5DB422-BF96-43DC-A9BA-12634A4F2BBC}" name="AT" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{EE047B0A-B831-48AA-B73B-E1927AF8CC86}" name="AP" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{C513E1E7-AAE7-4E76-9F05-8997EF765B3F}" name="AE" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{C8FF95F3-B743-4CF1-BB31-5218A0DEB0E2}" name="AV" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{E65FE900-9015-483F-BD63-03E8F53E8070}" name="NOME" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{83B8989C-17F6-4ED6-98C3-45E8D442FFE7}" name="CR" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{027923F2-5900-43B1-A215-2A9BC846F14C}" name="SL/B" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{DF7BF826-9991-4443-82C2-9826A1B4EDBC}" name="ET" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{D1A1A381-59C2-4080-BEF8-40B8E70D1796}" name="PROFESSOR" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{ADC459DE-BDC9-454A-824A-24BCD3A9031B}" name="ALUNOS MATRIC" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{9CD2D2FA-51BA-4A30-A0C5-D56FD2E46138}" name="DISCIPLINA" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{2A5DB422-BF96-43DC-A9BA-12634A4F2BBC}" name="AT" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{EE047B0A-B831-48AA-B73B-E1927AF8CC86}" name="AP" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{C513E1E7-AAE7-4E76-9F05-8997EF765B3F}" name="AE" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{C8FF95F3-B743-4CF1-BB31-5218A0DEB0E2}" name="AV" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{E65FE900-9015-483F-BD63-03E8F53E8070}" name="NOME" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{83B8989C-17F6-4ED6-98C3-45E8D442FFE7}" name="CR" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{027923F2-5900-43B1-A215-2A9BC846F14C}" name="SL/B" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{DF7BF826-9991-4443-82C2-9826A1B4EDBC}" name="ET" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{D1A1A381-59C2-4080-BEF8-40B8E70D1796}" name="PROFESSOR" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{ADC459DE-BDC9-454A-824A-24BCD3A9031B}" name="ALUNOS MATRIC" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{94BB9D13-CA19-4CA7-94BE-33C56E1E2F75}" name="Table16" displayName="Table16" ref="B44:L77" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{94BB9D13-CA19-4CA7-94BE-33C56E1E2F75}" name="Table16" displayName="Table16" ref="B44:L77" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="B44:L77" xr:uid="{94BB9D13-CA19-4CA7-94BE-33C56E1E2F75}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B45:L77">
     <sortCondition ref="B4:B42"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{706AB578-0B6F-43D3-BB61-D3E63C94C5C5}" name="DISCIPLINA" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{92C94A86-2FEF-421A-9CC5-CA7D417108D9}" name="AT" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{9907E328-02FC-4373-9361-D2E3BFE226DC}" name="AP" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{A7CC33C0-52CA-4582-8FF1-FEFEAE72EB0E}" name="AE" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{D8AFF64B-A3E3-413C-849B-0F0D3870941F}" name="AV" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{0CF01315-BEA4-4A80-9E81-286A7F94C7FA}" name="NOME" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{609DFCD0-358B-4053-86D5-D40C402E2F98}" name="CR" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{CD3E01FB-E340-4977-B45E-4E889CC1EAFA}" name="SL/B" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{6673106B-E091-46CB-9070-C0EE46C9E65E}" name="ET" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{26E42379-0ED6-41FA-A822-65DF2989814F}" name="PROFESSOR" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{1D04ED35-AD87-4382-977E-E166AC54C0B0}" name="ALUNOS MATRIC" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{706AB578-0B6F-43D3-BB61-D3E63C94C5C5}" name="DISCIPLINA" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{92C94A86-2FEF-421A-9CC5-CA7D417108D9}" name="AT" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{9907E328-02FC-4373-9361-D2E3BFE226DC}" name="AP" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{A7CC33C0-52CA-4582-8FF1-FEFEAE72EB0E}" name="AE" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{D8AFF64B-A3E3-413C-849B-0F0D3870941F}" name="AV" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{0CF01315-BEA4-4A80-9E81-286A7F94C7FA}" name="NOME" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{609DFCD0-358B-4053-86D5-D40C402E2F98}" name="CR" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{CD3E01FB-E340-4977-B45E-4E889CC1EAFA}" name="SL/B" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{6673106B-E091-46CB-9070-C0EE46C9E65E}" name="ET" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{26E42379-0ED6-41FA-A822-65DF2989814F}" name="PROFESSOR" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{1D04ED35-AD87-4382-977E-E166AC54C0B0}" name="ALUNOS MATRIC" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}" name="Table167" displayName="Table167" ref="A1:K34" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}" name="Table167" displayName="Table167" ref="A1:K34" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:K34" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K34">
     <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{99E45A2F-9332-4CFA-9CF0-E4A298DC69DF}" name="DISCIPLINA" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{4173FD76-8105-47F9-9DCE-D3B021A0F29D}" name="AT" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{8F80F768-1203-466E-B79F-E0C4F4AFAAB8}" name="AP" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{78918C4C-9168-4FAB-A2E3-24E3F8D870F8}" name="AE" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{B5F37458-7439-4148-8012-8EB48E3DD8D0}" name="AV" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{6F7EA491-05CE-4E0D-8968-65BA2793D6E8}" name="NOME" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{20008DE3-D13C-44CF-8CAA-58EC6DDABBBC}" name="CR" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{6789E295-1ACD-4B11-A4F9-01F3CECC14FA}" name="SL/B" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{509CA827-6B56-4C16-9CB0-D43DB4AF1E43}" name="ET" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{CC966D57-ACED-4B16-9CB1-406220269B5E}" name="PROFESSOR" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{20302694-742B-4E98-81D5-F6BA62536451}" name="ALUNOS MATRIC" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{99E45A2F-9332-4CFA-9CF0-E4A298DC69DF}" name="DISCIPLINA" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{4173FD76-8105-47F9-9DCE-D3B021A0F29D}" name="AT" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{8F80F768-1203-466E-B79F-E0C4F4AFAAB8}" name="AP" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{78918C4C-9168-4FAB-A2E3-24E3F8D870F8}" name="AE" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{B5F37458-7439-4148-8012-8EB48E3DD8D0}" name="AV" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{6F7EA491-05CE-4E0D-8968-65BA2793D6E8}" name="NOME" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{20008DE3-D13C-44CF-8CAA-58EC6DDABBBC}" name="CR" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{6789E295-1ACD-4B11-A4F9-01F3CECC14FA}" name="SL/B" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{509CA827-6B56-4C16-9CB0-D43DB4AF1E43}" name="ET" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{CC966D57-ACED-4B16-9CB1-406220269B5E}" name="PROFESSOR" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{20302694-742B-4E98-81D5-F6BA62536451}" name="ALUNOS MATRIC" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1235,7 +1268,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DA2ECD09-3FA6-4544-AE27-6E4A1304C0F4}" name="DISCIPLINA"/>
     <tableColumn id="2" xr3:uid="{C1D61556-D79E-4B3D-AE1A-582127EF40D7}" name="NOME"/>
-    <tableColumn id="3" xr3:uid="{0169D052-F3EC-453E-B9FA-D7EB40423470}" name="PROFESSOR CODE" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{0169D052-F3EC-453E-B9FA-D7EB40423470}" name="PROFESSOR CODE" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1248,7 +1281,7 @@
     <sortCondition ref="B4:B19"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BAE49131-A56E-44EB-BD41-330691452D20}" name="CODE" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{BAE49131-A56E-44EB-BD41-330691452D20}" name="CODE" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{EC56BC82-9C5A-473A-9BF8-799826212E29}" name="NOME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1256,53 +1289,27 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}" name="Table4" displayName="Table4" ref="I2:L35" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="I2:L35" xr:uid="{04C15787-7303-4E28-8F4C-E1FD2B94BF16}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:L35">
-    <sortCondition ref="L2:L35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2991064F-D415-454C-8AB0-8A1746C4F778}" name="Table1678" displayName="Table1678" ref="B2:M36" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="B2:M35" xr:uid="{2991064F-D415-454C-8AB0-8A1746C4F778}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M35">
+    <sortCondition ref="J2:J35"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C8A0A278-3838-4995-8588-B07D13EA3EFD}" name="NOME" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{D7D84DAB-D2AE-4879-9CEE-32E7CA42BC4C}" name="CR" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{60337C39-789F-4651-A8AB-E68BD1E538E3}" name="SL/B" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{4DEB40D6-B26B-4C55-8BD0-3BE4E24E00B0}" name="ET" dataDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{481FA10C-0BC0-4E91-B80D-8591478485CF}" name="Table18" displayName="Table18" ref="B38:L53" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="B38:L53" xr:uid="{481FA10C-0BC0-4E91-B80D-8591478485CF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B39:L53">
-    <sortCondition ref="K38:K53"/>
-  </sortState>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F372217B-2A68-4004-9285-10D7E90A0B0E}" name="DISCIPLINA" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C3BB104A-81EF-4C52-A9A7-530A07856212}" name="AT" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{9B4C9EEB-F5DD-482F-95C3-C29CAEFFAC7E}" name="AP" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{96A7B98D-1D2D-44E9-8260-91F05512BE0F}" name="AE" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{D4B47FCE-9802-417E-9CFB-9D6A58D0BACD}" name="AV" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{F9B14BF4-A785-46B9-A7D3-7B536EE599CC}" name="NOME" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{1E7008A2-4E60-4A02-A858-067C78FF6A22}" name="CR" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{667FADCE-6DFF-44D9-AB54-CD21B2BDF7F0}" name="SL/B" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{2D307CC2-649E-4D1E-91FA-80EE15A24E37}" name="ET" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{E92D9F71-5E60-4BCC-A870-768E44959260}" name="PROFESSOR" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{BF05BD94-4998-4F11-8493-3B000AE8928B}" name="ALUNOS MATRIC" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C94CF6EC-5DC4-4F85-9B0C-70D8A6D701D3}" name="Table39" displayName="Table39" ref="N38:O53" totalsRowShown="0">
-  <autoFilter ref="N38:O53" xr:uid="{C94CF6EC-5DC4-4F85-9B0C-70D8A6D701D3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N39:O53">
-    <sortCondition ref="N4:N19"/>
-  </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F31A5C4C-7274-4461-9C86-51126542426E}" name="CODE" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{FBEE49C1-B9C9-4BCA-8857-9A5002D2147E}" name="NOME"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{6E76E4D0-CF80-40D0-ACBC-CF5766F1B002}" name="DISCIPLINA" dataDxfId="23" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4D25F4D0-39BD-48C0-91A2-3FE6DAE1B264}" name="AT" dataDxfId="22" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{BF646761-0536-4BC4-BAA8-38979D662958}" name="AP" dataDxfId="21" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{B137D78E-F0C9-4A47-9B90-77310FB82685}" name="AE" dataDxfId="20" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{FF836065-FDA0-4A8E-BAE3-D8266F68165B}" name="AV" dataDxfId="19" totalsRowDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{27B4B7E4-F7A5-46C7-BCB7-B059C85755B0}" name="NOME" dataDxfId="18" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{F970B31E-AA1A-4FEC-8AC3-63D847FF7B7F}" name="CR" dataDxfId="17" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{E88475F6-9C4E-44EE-9673-25791F5D5178}" name="SL/B" dataDxfId="16" totalsRowDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{37CDF4FD-7E30-47DF-8209-E35AE5093E86}" name="ET" dataDxfId="15" totalsRowDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{F289FC18-D622-4229-939B-52407423F01E}" name="PROFESSOR" dataDxfId="14" totalsRowDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{DF7095CA-F6C0-4997-AB69-746DA4C9C5A1}" name="ALUNOS MATRIC" dataDxfId="13" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{F0094D81-6F9E-418E-B741-7A7BB45F7A88}" name="Hours" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="0">
+      <calculatedColumnFormula>SUM(Table1678[[#This Row],[AT]:[AV]])</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Table1678[Hours])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1573,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L77"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,12 +1595,12 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -1632,7 +1639,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -1647,33 +1654,33 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
         <v>73</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2">
-        <v>45000</v>
+        <v>13070</v>
       </c>
       <c r="L5" s="5">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -1682,33 +1689,33 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
         <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2">
-        <v>14091</v>
+        <v>13070</v>
       </c>
       <c r="L6" s="5">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -1717,27 +1724,27 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
         <v>73</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2">
-        <v>13034</v>
+        <v>11785</v>
       </c>
       <c r="L7" s="5">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1752,33 +1759,33 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
         <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K8" s="2">
-        <v>14525</v>
+        <v>11785</v>
       </c>
       <c r="L8" s="5">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -1787,27 +1794,27 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H9" t="s">
         <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="J9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
-        <v>14642</v>
+        <v>11792</v>
       </c>
       <c r="L9" s="5">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1819,10 +1826,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="H10" t="s">
         <v>73</v>
@@ -1831,18 +1838,18 @@
         <v>77</v>
       </c>
       <c r="J10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
-        <v>12274</v>
+        <v>13034</v>
       </c>
       <c r="L10" s="5">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1857,30 +1864,30 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
         <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K11" s="2">
-        <v>14875</v>
+        <v>45000</v>
       </c>
       <c r="L11" s="5">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -1889,30 +1896,30 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
         <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K12" s="2">
-        <v>14525</v>
+        <v>45000</v>
       </c>
       <c r="L12" s="5">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1927,16 +1934,16 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H13" t="s">
         <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K13" s="2">
         <v>45000</v>
@@ -1947,13 +1954,13 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -1962,62 +1969,62 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="H14" t="s">
         <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K14" s="2">
-        <v>13000</v>
+        <v>11792</v>
       </c>
       <c r="L14" s="5">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="H15" t="s">
         <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K15" s="2">
-        <v>14525</v>
+        <v>14091</v>
       </c>
       <c r="L15" s="5">
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -2029,36 +2036,36 @@
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H16" t="s">
         <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K16" s="2">
-        <v>14642</v>
+        <v>12203</v>
       </c>
       <c r="L16" s="5">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -2067,33 +2074,33 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
         <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K17" s="2">
-        <v>14875</v>
+        <v>14472</v>
       </c>
       <c r="L17" s="5">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -2102,62 +2109,62 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
         <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K18" s="2">
-        <v>14616</v>
+        <v>14472</v>
       </c>
       <c r="L18" s="5">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19">
         <v>3</v>
       </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19">
-        <v>7</v>
-      </c>
       <c r="K19" s="2">
-        <v>13000</v>
+        <v>13034</v>
       </c>
       <c r="L19" s="5">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -2172,27 +2179,27 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="H20" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K20" s="2">
-        <v>13070</v>
+        <v>13034</v>
       </c>
       <c r="L20" s="5">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -2207,42 +2214,42 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="H21" t="s">
         <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J21">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K21" s="2">
         <v>14642</v>
       </c>
       <c r="L21" s="5">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="H22" t="s">
         <v>73</v>
@@ -2254,18 +2261,18 @@
         <v>3</v>
       </c>
       <c r="K22" s="2">
-        <v>14091</v>
+        <v>14472</v>
       </c>
       <c r="L22" s="5">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -2274,10 +2281,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
         <v>73</v>
@@ -2286,24 +2293,24 @@
         <v>76</v>
       </c>
       <c r="J23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K23" s="2">
-        <v>45000</v>
+        <v>14091</v>
       </c>
       <c r="L23" s="5">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -2312,68 +2319,68 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
         <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K24" s="2">
-        <v>45000</v>
+        <v>13034</v>
       </c>
       <c r="L24" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H25" t="s">
         <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="J25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K25" s="2">
-        <v>12203</v>
+        <v>14525</v>
       </c>
       <c r="L25" s="5">
-        <v>71</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -2382,27 +2389,27 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H26" t="s">
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K26" s="2">
-        <v>14472</v>
+        <v>14642</v>
       </c>
       <c r="L26" s="5">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -2417,27 +2424,27 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="H27" t="s">
         <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K27" s="2">
-        <v>14472</v>
+        <v>14642</v>
       </c>
       <c r="L27" s="5">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -2452,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="H28" t="s">
         <v>73</v>
@@ -2464,21 +2471,21 @@
         <v>5</v>
       </c>
       <c r="K28" s="2">
-        <v>14776</v>
+        <v>12274</v>
       </c>
       <c r="L28" s="5">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -2487,27 +2494,27 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="H29" t="s">
         <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J29">
         <v>5</v>
       </c>
       <c r="K29" s="2">
-        <v>13034</v>
+        <v>14875</v>
       </c>
       <c r="L29" s="5">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -2522,33 +2529,33 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="H30" t="s">
         <v>73</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K30" s="2">
-        <v>11792</v>
+        <v>14525</v>
       </c>
       <c r="L30" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -2557,33 +2564,33 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H31" t="s">
         <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K31" s="2">
-        <v>13070</v>
+        <v>14776</v>
       </c>
       <c r="L31" s="5">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -2592,27 +2599,27 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H32" t="s">
         <v>73</v>
       </c>
       <c r="I32" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K32" s="2">
-        <v>13070</v>
+        <v>13034</v>
       </c>
       <c r="L32" s="5">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -2627,27 +2634,27 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="H33" t="s">
         <v>73</v>
       </c>
       <c r="I33" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K33" s="2">
-        <v>11785</v>
+        <v>45000</v>
       </c>
       <c r="L33" s="5">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -2662,62 +2669,62 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
         <v>73</v>
       </c>
       <c r="I34" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K34" s="2">
-        <v>11785</v>
+        <v>13000</v>
       </c>
       <c r="L34" s="5">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J35">
+        <v>6</v>
+      </c>
+      <c r="K35" s="2">
+        <v>14525</v>
+      </c>
+      <c r="L35" s="5">
         <v>4</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-      <c r="G35" t="s">
-        <v>127</v>
-      </c>
-      <c r="H35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" t="s">
-        <v>86</v>
-      </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35" s="2">
-        <v>11792</v>
-      </c>
-      <c r="L35" s="5">
-        <v>52</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
@@ -2729,36 +2736,36 @@
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
       <c r="H36" t="s">
         <v>73</v>
       </c>
       <c r="I36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K36" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
       <c r="L36" s="5">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -2767,27 +2774,27 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="H37" t="s">
         <v>73</v>
       </c>
       <c r="I37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J37">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K37" s="2">
-        <v>13034</v>
+        <v>14875</v>
       </c>
       <c r="L37" s="5">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
@@ -2802,33 +2809,33 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="H38" t="s">
         <v>73</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J38">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K38" s="2">
-        <v>13034</v>
+        <v>14616</v>
       </c>
       <c r="L38" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C39" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -2837,27 +2844,27 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="H39" t="s">
         <v>73</v>
       </c>
       <c r="I39" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J39">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K39" s="2">
-        <v>14642</v>
+        <v>13000</v>
       </c>
       <c r="L39" s="5">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
@@ -2872,27 +2879,27 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="H40" t="s">
         <v>73</v>
       </c>
       <c r="I40" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K40" s="2">
-        <v>14472</v>
+        <v>13070</v>
       </c>
       <c r="L40" s="5">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
@@ -2907,33 +2914,33 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H41" t="s">
         <v>73</v>
       </c>
       <c r="I41" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K41" s="2">
         <v>11792</v>
       </c>
       <c r="L41" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -2942,22 +2949,22 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H42" t="s">
         <v>73</v>
       </c>
       <c r="I42" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K42" s="2">
         <v>14642</v>
       </c>
       <c r="L42" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
@@ -4167,8 +4174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C694DF4-CEA0-4BF6-94BA-E896B085E534}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5375,7 +5382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177CF1B3-023B-4C26-8BA7-3BF936A39EC1}">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -5391,10 +5398,10 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -5960,12 +5967,12 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
@@ -6127,1257 +6134,1364 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71808F-48CA-4498-917A-4D75806DE602}">
-  <dimension ref="B2:O53"/>
+  <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="H2" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="I2" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="J2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="K2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>13070</v>
+      </c>
+      <c r="L3" s="5">
+        <v>61</v>
+      </c>
+      <c r="M3" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>11785</v>
+      </c>
+      <c r="L4" s="5">
+        <v>56</v>
+      </c>
+      <c r="M4" s="12">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>11792</v>
+      </c>
+      <c r="L5" s="5">
+        <v>52</v>
+      </c>
+      <c r="M5" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>13034</v>
+      </c>
+      <c r="L6" s="5">
+        <v>59</v>
+      </c>
+      <c r="M6" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>45000</v>
+      </c>
+      <c r="L7" s="5">
+        <v>2</v>
+      </c>
+      <c r="M7" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>45000</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>45000</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>11792</v>
+      </c>
+      <c r="L10" s="5">
+        <v>18</v>
+      </c>
+      <c r="M10" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>14091</v>
+      </c>
+      <c r="L11" s="5">
+        <v>53</v>
+      </c>
+      <c r="M11" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>12203</v>
+      </c>
+      <c r="L12" s="5">
+        <v>71</v>
+      </c>
+      <c r="M12" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="L4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13" s="2">
+        <v>14472</v>
+      </c>
+      <c r="L13" s="5">
+        <v>61</v>
+      </c>
+      <c r="M13" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>13034</v>
+      </c>
+      <c r="L14" s="5">
+        <v>50</v>
+      </c>
+      <c r="M14" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15" s="2">
+        <v>14472</v>
+      </c>
+      <c r="L15" s="5">
+        <v>56</v>
+      </c>
+      <c r="M15" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>14091</v>
+      </c>
+      <c r="L16" s="5">
+        <v>14</v>
+      </c>
+      <c r="M16" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>13034</v>
+      </c>
+      <c r="L17" s="5">
+        <v>11</v>
+      </c>
+      <c r="M17" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>14525</v>
+      </c>
+      <c r="L18" s="5">
+        <v>10</v>
+      </c>
+      <c r="M18" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>14642</v>
+      </c>
+      <c r="L19" s="5">
+        <v>11</v>
+      </c>
+      <c r="M19" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20" s="2">
+        <v>14642</v>
+      </c>
+      <c r="L20" s="5">
+        <v>20</v>
+      </c>
+      <c r="M20" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21" s="2">
+        <v>12274</v>
+      </c>
+      <c r="L21" s="5">
+        <v>27</v>
+      </c>
+      <c r="M21" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>14875</v>
+      </c>
+      <c r="L22" s="5">
+        <v>16</v>
+      </c>
+      <c r="M22" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23" s="2">
+        <v>14525</v>
+      </c>
+      <c r="L23" s="5">
+        <v>21</v>
+      </c>
+      <c r="M23" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24" s="2">
+        <v>14776</v>
+      </c>
+      <c r="L24" s="5">
+        <v>17</v>
+      </c>
+      <c r="M24" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25" s="2">
+        <v>13034</v>
+      </c>
+      <c r="L25" s="5">
+        <v>27</v>
+      </c>
+      <c r="M25" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="H26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26" s="2">
+        <v>45000</v>
+      </c>
+      <c r="L26" s="5">
+        <v>1</v>
+      </c>
+      <c r="M26" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="K27" s="2">
+        <v>13000</v>
+      </c>
+      <c r="L27" s="5">
+        <v>6</v>
+      </c>
+      <c r="M27" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28">
+        <v>6</v>
+      </c>
+      <c r="K28" s="2">
+        <v>14525</v>
+      </c>
+      <c r="L28" s="5">
+        <v>4</v>
+      </c>
+      <c r="M28" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+      <c r="K29" s="2">
+        <v>14642</v>
+      </c>
+      <c r="L29" s="5">
+        <v>18</v>
+      </c>
+      <c r="M29" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30">
+        <v>7</v>
+      </c>
+      <c r="K30" s="2">
+        <v>14875</v>
+      </c>
+      <c r="L30" s="5">
+        <v>18</v>
+      </c>
+      <c r="M30" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="L6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="L7" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="L8" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K9" s="6" t="s">
+      <c r="H31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" t="s">
+        <v>80</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31" s="2">
+        <v>14616</v>
+      </c>
+      <c r="L31" s="5">
+        <v>22</v>
+      </c>
+      <c r="M31" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32">
+        <v>7</v>
+      </c>
+      <c r="K32" s="2">
+        <v>13000</v>
+      </c>
+      <c r="L32" s="5">
+        <v>19</v>
+      </c>
+      <c r="M32" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L11" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L12" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="L13" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L15" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="L16" s="6">
+      <c r="J33">
+        <v>7</v>
+      </c>
+      <c r="K33" s="2">
+        <v>13070</v>
+      </c>
+      <c r="L33" s="5">
+        <v>14</v>
+      </c>
+      <c r="M33" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="L17" s="7">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" s="6">
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34">
+        <v>7</v>
+      </c>
+      <c r="K34" s="2">
+        <v>11792</v>
+      </c>
+      <c r="L34" s="5">
+        <v>22</v>
+      </c>
+      <c r="M34" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="L19" s="7">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35">
+        <v>8</v>
+      </c>
+      <c r="K35" s="2">
+        <v>14642</v>
+      </c>
+      <c r="L35" s="5">
+        <v>12</v>
+      </c>
+      <c r="M35" s="9">
+        <f>SUM(Table1678[[#This Row],[AT]:[AV]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="L20" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L21" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="L22" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L23" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L24" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L25" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L26" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L27" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L28" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L29" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L30" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L31" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L32" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="L33" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="L34" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L35" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" t="s">
-        <v>44</v>
-      </c>
-      <c r="H38" t="s">
-        <v>72</v>
-      </c>
-      <c r="I38" t="s">
-        <v>74</v>
-      </c>
-      <c r="J38" t="s">
-        <v>88</v>
-      </c>
-      <c r="K38" t="s">
-        <v>89</v>
-      </c>
-      <c r="L38" t="s">
-        <v>105</v>
-      </c>
-      <c r="N38" t="s">
-        <v>144</v>
-      </c>
-      <c r="O38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="1">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1">
-        <v>0</v>
-      </c>
-      <c r="G39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H39" t="s">
-        <v>73</v>
-      </c>
-      <c r="I39" t="s">
-        <v>86</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39" s="2">
-        <v>11785</v>
-      </c>
-      <c r="L39" s="5">
-        <v>26</v>
-      </c>
-      <c r="N39" s="4">
-        <v>11785</v>
-      </c>
-      <c r="O39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="1">
-        <v>4</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>129</v>
-      </c>
-      <c r="H40" t="s">
-        <v>73</v>
-      </c>
-      <c r="I40" t="s">
-        <v>85</v>
-      </c>
-      <c r="J40">
-        <v>7</v>
-      </c>
-      <c r="K40" s="2">
-        <v>11792</v>
-      </c>
-      <c r="L40" s="5">
-        <v>22</v>
-      </c>
-      <c r="N40" s="4">
-        <v>11792</v>
-      </c>
-      <c r="O40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="1">
-        <v>2</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
-      <c r="F41" s="1">
-        <v>2</v>
-      </c>
-      <c r="G41" t="s">
-        <v>63</v>
-      </c>
-      <c r="H41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I41" t="s">
-        <v>84</v>
-      </c>
-      <c r="J41">
-        <v>3</v>
-      </c>
-      <c r="K41" s="2">
-        <v>12203</v>
-      </c>
-      <c r="L41" s="5">
-        <v>71</v>
-      </c>
-      <c r="N41" s="4">
-        <v>12203</v>
-      </c>
-      <c r="O41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="1">
-        <v>2</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" t="s">
-        <v>49</v>
-      </c>
-      <c r="H42" t="s">
-        <v>73</v>
-      </c>
-      <c r="I42" t="s">
-        <v>77</v>
-      </c>
-      <c r="J42">
-        <v>5</v>
-      </c>
-      <c r="K42" s="2">
-        <v>12274</v>
-      </c>
-      <c r="L42" s="5">
-        <v>27</v>
-      </c>
-      <c r="N42" s="4">
-        <v>12274</v>
-      </c>
-      <c r="O42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="1">
-        <v>2</v>
-      </c>
-      <c r="D43" s="1">
-        <v>2</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-      <c r="F43" s="1">
-        <v>0</v>
-      </c>
-      <c r="G43" t="s">
-        <v>53</v>
-      </c>
-      <c r="H43" t="s">
-        <v>73</v>
-      </c>
-      <c r="I43" t="s">
-        <v>81</v>
-      </c>
-      <c r="J43">
-        <v>6</v>
-      </c>
-      <c r="K43" s="2">
-        <v>13000</v>
-      </c>
-      <c r="L43" s="5">
-        <v>6</v>
-      </c>
-      <c r="N43" s="4">
-        <v>13000</v>
-      </c>
-      <c r="O43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-      <c r="F44" s="1">
-        <v>0</v>
-      </c>
-      <c r="G44" t="s">
-        <v>47</v>
-      </c>
-      <c r="H44" t="s">
-        <v>73</v>
-      </c>
-      <c r="I44" t="s">
-        <v>76</v>
-      </c>
-      <c r="J44">
-        <v>4</v>
-      </c>
-      <c r="K44" s="2">
-        <v>13034</v>
-      </c>
-      <c r="L44" s="5">
-        <v>11</v>
-      </c>
-      <c r="N44" s="4">
-        <v>13034</v>
-      </c>
-      <c r="O44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="1">
-        <v>2</v>
-      </c>
-      <c r="D45" s="1">
-        <v>2</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-      <c r="F45" s="1">
-        <v>0</v>
-      </c>
-      <c r="G45" t="s">
-        <v>58</v>
-      </c>
-      <c r="H45" t="s">
-        <v>73</v>
-      </c>
-      <c r="I45" t="s">
-        <v>75</v>
-      </c>
-      <c r="J45">
-        <v>7</v>
-      </c>
-      <c r="K45" s="2">
-        <v>13070</v>
-      </c>
-      <c r="L45" s="5">
-        <v>14</v>
-      </c>
-      <c r="N45" s="4">
-        <v>13070</v>
-      </c>
-      <c r="O45" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="1">
-        <v>2</v>
-      </c>
-      <c r="D46" s="1">
-        <v>0</v>
-      </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
-      <c r="F46" s="1">
-        <v>0</v>
-      </c>
-      <c r="G46" t="s">
-        <v>46</v>
-      </c>
-      <c r="H46" t="s">
-        <v>73</v>
-      </c>
-      <c r="I46" t="s">
-        <v>76</v>
-      </c>
-      <c r="J46">
-        <v>4</v>
-      </c>
-      <c r="K46" s="2">
-        <v>14091</v>
-      </c>
-      <c r="L46" s="5">
-        <v>14</v>
-      </c>
-      <c r="N46" s="4">
-        <v>14091</v>
-      </c>
-      <c r="O46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="1">
-        <v>3</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-      <c r="F47" s="1">
-        <v>0</v>
-      </c>
-      <c r="G47" t="s">
-        <v>64</v>
-      </c>
-      <c r="H47" t="s">
-        <v>73</v>
-      </c>
-      <c r="I47" t="s">
-        <v>79</v>
-      </c>
-      <c r="J47">
-        <v>3</v>
-      </c>
-      <c r="K47" s="2">
-        <v>14472</v>
-      </c>
-      <c r="L47" s="5">
-        <v>28</v>
-      </c>
-      <c r="N47" s="4">
-        <v>14472</v>
-      </c>
-      <c r="O47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1">
-        <v>2</v>
-      </c>
-      <c r="D48" s="1">
-        <v>2</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-      <c r="F48" s="1">
-        <v>0</v>
-      </c>
-      <c r="G48" t="s">
-        <v>48</v>
-      </c>
-      <c r="H48" t="s">
-        <v>73</v>
-      </c>
-      <c r="I48" t="s">
-        <v>76</v>
-      </c>
-      <c r="J48">
-        <v>4</v>
-      </c>
-      <c r="K48" s="2">
-        <v>14525</v>
-      </c>
-      <c r="L48" s="5">
-        <v>10</v>
-      </c>
-      <c r="N48" s="4">
-        <v>14525</v>
-      </c>
-      <c r="O48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="1">
-        <v>2</v>
-      </c>
-      <c r="D49" s="1">
-        <v>2</v>
-      </c>
-      <c r="E49" s="1">
-        <v>0</v>
-      </c>
-      <c r="F49" s="1">
-        <v>0</v>
-      </c>
-      <c r="G49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H49" t="s">
-        <v>73</v>
-      </c>
-      <c r="I49" t="s">
-        <v>80</v>
-      </c>
-      <c r="J49">
-        <v>7</v>
-      </c>
-      <c r="K49" s="2">
-        <v>14616</v>
-      </c>
-      <c r="L49" s="5">
-        <v>22</v>
-      </c>
-      <c r="N49" s="4">
-        <v>14616</v>
-      </c>
-      <c r="O49" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="1">
-        <v>3</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1">
-        <v>0</v>
-      </c>
-      <c r="F50" s="1">
-        <v>0</v>
-      </c>
-      <c r="G50" t="s">
-        <v>123</v>
-      </c>
-      <c r="H50" t="s">
-        <v>73</v>
-      </c>
-      <c r="I50" t="s">
-        <v>77</v>
-      </c>
-      <c r="J50">
-        <v>5</v>
-      </c>
-      <c r="K50" s="2">
-        <v>14642</v>
-      </c>
-      <c r="L50" s="5">
-        <v>20</v>
-      </c>
-      <c r="N50" s="4">
-        <v>14642</v>
-      </c>
-      <c r="O50" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" s="1">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-      <c r="F51" s="1">
-        <v>0</v>
-      </c>
-      <c r="G51" t="s">
-        <v>65</v>
-      </c>
-      <c r="H51" t="s">
-        <v>73</v>
-      </c>
-      <c r="I51" t="s">
-        <v>77</v>
-      </c>
-      <c r="J51">
-        <v>5</v>
-      </c>
-      <c r="K51" s="2">
-        <v>14776</v>
-      </c>
-      <c r="L51" s="5">
-        <v>17</v>
-      </c>
-      <c r="N51" s="4">
-        <v>14776</v>
-      </c>
-      <c r="O51" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="1">
-        <v>2</v>
-      </c>
-      <c r="D52" s="1">
-        <v>2</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="1">
-        <v>0</v>
-      </c>
-      <c r="G52" t="s">
-        <v>50</v>
-      </c>
-      <c r="H52" t="s">
-        <v>73</v>
-      </c>
-      <c r="I52" t="s">
-        <v>78</v>
-      </c>
-      <c r="J52">
-        <v>5</v>
-      </c>
-      <c r="K52" s="2">
-        <v>14875</v>
-      </c>
-      <c r="L52" s="5">
-        <v>16</v>
-      </c>
-      <c r="N52" s="4">
-        <v>14875</v>
-      </c>
-      <c r="O52" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53" s="1">
-        <v>2</v>
-      </c>
-      <c r="D53" s="1">
-        <v>2</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="F53" s="1">
-        <v>0</v>
-      </c>
-      <c r="G53" t="s">
-        <v>45</v>
-      </c>
-      <c r="H53" t="s">
-        <v>73</v>
-      </c>
-      <c r="I53" t="s">
-        <v>75</v>
-      </c>
-      <c r="J53">
-        <v>2</v>
-      </c>
-      <c r="K53" s="2">
-        <v>45000</v>
-      </c>
-      <c r="L53" s="5">
-        <v>2</v>
-      </c>
-      <c r="N53" s="4">
-        <v>45000</v>
-      </c>
-      <c r="O53" t="s">
-        <v>96</v>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="12">
+        <f>SUM(Table1678[Hours])</f>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented the local search
</commit_message>
<xml_diff>
--- a/data/Curso Engenharia de software.xlsx
+++ b/data/Curso Engenharia de software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a5892ed9debdf/Documents/Semester5en6/Stage/Genetic_alg_internship/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1192" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E4FFBA3-1643-41F5-AD03-B87A7E3C7078}"/>
+  <xr:revisionPtr revIDLastSave="1193" documentId="11_AD4DB114E441178AC67DF46F4610FAEE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7315946A-227A-4DC1-A5F9-BA723BC7967A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Schedule" sheetId="1" r:id="rId1"/>
@@ -1493,7 +1493,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}" name="Table167" displayName="Table167" ref="A1:L35" totalsRowCount="1" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:L34" xr:uid="{152BE743-8563-4F90-BF1C-05322D60DE35}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L34">
-    <sortCondition ref="I1:I34"/>
+    <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{99E45A2F-9332-4CFA-9CF0-E4A298DC69DF}" name="DISCIPLINA" dataDxfId="57" totalsRowDxfId="56"/>
@@ -4459,8 +4459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C694DF4-CEA0-4BF6-94BA-E896B085E534}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -4520,22 +4520,22 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
         <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" s="2">
-        <v>13070</v>
+        <v>45000</v>
       </c>
       <c r="K2" s="5">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="L2">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
@@ -4544,13 +4544,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -4559,115 +4559,115 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
         <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J3" s="2">
-        <v>11785</v>
+        <v>14091</v>
       </c>
       <c r="K3" s="5">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="L3">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4" s="2">
-        <v>11792</v>
+        <v>13034</v>
       </c>
       <c r="K4" s="5">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="L4">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
         <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J5" s="2">
-        <v>13034</v>
+        <v>14525</v>
       </c>
       <c r="K5" s="5">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="L5">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -4676,34 +4676,34 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
         <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J6" s="2">
-        <v>45000</v>
+        <v>14642</v>
       </c>
       <c r="K6" s="5">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="L6">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -4712,34 +4712,34 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
         <v>73</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J7" s="2">
-        <v>45000</v>
+        <v>12274</v>
       </c>
       <c r="K7" s="5">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="L7">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -4754,31 +4754,31 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J8" s="2">
-        <v>45000</v>
+        <v>14875</v>
       </c>
       <c r="K8" s="5">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="L8">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -4793,112 +4793,112 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J9" s="2">
-        <v>11792</v>
+        <v>14525</v>
       </c>
       <c r="K9" s="5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L9">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s">
         <v>73</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J10" s="2">
-        <v>14091</v>
+        <v>45000</v>
       </c>
       <c r="K10" s="5">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J11" s="2">
-        <v>12203</v>
+        <v>13000</v>
       </c>
       <c r="K11" s="5">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="L11">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -4910,37 +4910,37 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J12" s="2">
-        <v>14472</v>
+        <v>14525</v>
       </c>
       <c r="K12" s="5">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="L12">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -4949,37 +4949,37 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
         <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J13" s="2">
-        <v>13034</v>
+        <v>14642</v>
       </c>
       <c r="K13" s="5">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="L13">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -4988,37 +4988,37 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
         <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J14" s="2">
-        <v>14472</v>
+        <v>14875</v>
       </c>
       <c r="K14" s="5">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="L14">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -5027,34 +5027,34 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="G15" t="s">
         <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J15" s="2">
-        <v>14091</v>
+        <v>14616</v>
       </c>
       <c r="K15" s="5">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="L15">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -5066,31 +5066,31 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G16" t="s">
         <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J16" s="2">
-        <v>13034</v>
+        <v>13000</v>
       </c>
       <c r="K16" s="5">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L16">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -5105,22 +5105,22 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G17" t="s">
         <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J17" s="2">
-        <v>14525</v>
+        <v>13070</v>
       </c>
       <c r="K17" s="5">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L17">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
@@ -5129,13 +5129,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -5144,22 +5144,22 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
         <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J18" s="2">
         <v>14642</v>
       </c>
       <c r="K18" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L18">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
@@ -5168,49 +5168,49 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19">
         <v>3</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19">
-        <v>5</v>
-      </c>
       <c r="J19" s="2">
-        <v>14642</v>
+        <v>14091</v>
       </c>
       <c r="K19" s="5">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="L19">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -5219,34 +5219,34 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
         <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J20" s="2">
-        <v>12274</v>
+        <v>45000</v>
       </c>
       <c r="K20" s="5">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="L20">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -5261,34 +5261,34 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
         <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J21" s="2">
-        <v>14875</v>
+        <v>45000</v>
       </c>
       <c r="K21" s="5">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -5297,40 +5297,40 @@
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
         <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J22" s="2">
-        <v>14525</v>
+        <v>12203</v>
       </c>
       <c r="K22" s="5">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="L22">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -5339,37 +5339,37 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" t="s">
         <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J23" s="2">
-        <v>14776</v>
+        <v>14472</v>
       </c>
       <c r="K23" s="5">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="L23">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -5378,37 +5378,37 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
         <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I24">
         <v>5</v>
       </c>
       <c r="J24" s="2">
-        <v>13034</v>
+        <v>14776</v>
       </c>
       <c r="K24" s="5">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="L24">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -5417,22 +5417,22 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="G25" t="s">
         <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J25" s="2">
-        <v>45000</v>
+        <v>13034</v>
       </c>
       <c r="K25" s="5">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="L25">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
@@ -5441,13 +5441,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B26" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -5456,22 +5456,22 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="G26" t="s">
         <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J26" s="2">
-        <v>13000</v>
+        <v>11792</v>
       </c>
       <c r="K26" s="5">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="L26">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
@@ -5480,52 +5480,52 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I27">
         <v>1</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" t="s">
-        <v>82</v>
-      </c>
-      <c r="I27">
-        <v>6</v>
-      </c>
       <c r="J27" s="2">
-        <v>14525</v>
+        <v>13070</v>
       </c>
       <c r="K27" s="5">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="L27">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -5534,34 +5534,34 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="G28" t="s">
         <v>73</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I28">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J28" s="2">
-        <v>14642</v>
+        <v>11785</v>
       </c>
       <c r="K28" s="5">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="L28">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -5573,109 +5573,109 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="G29" t="s">
         <v>73</v>
       </c>
       <c r="H29" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J29" s="2">
-        <v>14875</v>
+        <v>11792</v>
       </c>
       <c r="K29" s="5">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="L29">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="G30" t="s">
         <v>73</v>
       </c>
       <c r="H30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I30">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J30" s="2">
-        <v>14616</v>
+        <v>13034</v>
       </c>
       <c r="K30" s="5">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="L30">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31">
         <v>3</v>
       </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" t="s">
-        <v>73</v>
-      </c>
-      <c r="H31" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31">
-        <v>7</v>
-      </c>
       <c r="J31" s="2">
-        <v>13000</v>
+        <v>13034</v>
       </c>
       <c r="K31" s="5">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="L31">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="B32" s="1">
         <v>2</v>
@@ -5690,31 +5690,31 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
         <v>73</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J32" s="2">
-        <v>13070</v>
+        <v>14472</v>
       </c>
       <c r="K32" s="5">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="L32">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
@@ -5729,37 +5729,37 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G33" t="s">
         <v>73</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I33">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J33" s="2">
         <v>11792</v>
       </c>
       <c r="K33" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L33">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -5768,22 +5768,22 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G34" t="s">
         <v>73</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="I34">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J34" s="2">
         <v>14642</v>
       </c>
       <c r="K34" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L34">
         <f>IF(Table167[[#This Row],[ET]]&lt;4,2*SUM(Table167[[#This Row],[AT]:[AV]]),SUM(Table167[[#This Row],[AT]:[AV]]))</f>
@@ -5813,7 +5813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177CF1B3-023B-4C26-8BA7-3BF936A39EC1}">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>